<commit_message>
+ Home Section 1
</commit_message>
<xml_diff>
--- a/data/text.xlsx
+++ b/data/text.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\ReactJS\_neko_website\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB58E43-A821-4A11-B540-DE502160D430}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9049BF7-2C57-42ED-8D6A-66BD4836C28B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3930" yWindow="3540" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COMMON" sheetId="1" r:id="rId1"/>
@@ -305,12 +305,39 @@
 through understanding the user experience.</t>
   </si>
   <si>
-    <t>&lt;span style="color:blue"&gt;We make it live.&lt;/span&gt;</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Big idea to create your
 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;span className='{{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>custom</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>}}'&gt;</t>
     </r>
     <r>
       <rPr>
@@ -320,7 +347,69 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>&lt;span {{styles}}&gt;brand personality&lt;/span&gt;</t>
+      <t>brand personality</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;/span&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;span className='{{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>custom</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>}}'&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFF26A65"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>We make it live.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;/span&gt;</t>
     </r>
   </si>
 </sst>
@@ -328,7 +417,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -357,6 +446,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -724,7 +827,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1156,13 +1259,13 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="46.7109375" customWidth="1"/>
+    <col min="2" max="2" width="56.28515625" customWidth="1"/>
     <col min="3" max="3" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1182,7 +1285,7 @@
         <v>85</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1190,7 +1293,7 @@
         <v>86</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
+ Home section 2
</commit_message>
<xml_diff>
--- a/data/text.xlsx
+++ b/data/text.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\ReactJS\_neko_website\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2569199-74CF-4E8C-B8A6-F353EBD106A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC96701-BB55-48FD-82E1-35C492074E7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3930" yWindow="3540" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3930" yWindow="3540" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COMMON" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="124">
   <si>
     <t>::ID::</t>
   </si>
@@ -436,6 +436,69 @@
   </si>
   <si>
     <t>https://www.youtube.com</t>
+  </si>
+  <si>
+    <t>SECTION_2_TEXT_1</t>
+  </si>
+  <si>
+    <t>we specialized in</t>
+  </si>
+  <si>
+    <t>SECTION_2_MENU_1</t>
+  </si>
+  <si>
+    <t>SECTION_2_MENU_2</t>
+  </si>
+  <si>
+    <t>SECTION_2_MENU_3</t>
+  </si>
+  <si>
+    <t>SECTION_2_MENU_4</t>
+  </si>
+  <si>
+    <t>SECTION_2_MENU_5</t>
+  </si>
+  <si>
+    <t>Brand identity</t>
+  </si>
+  <si>
+    <t>User Interface</t>
+  </si>
+  <si>
+    <t>WORKS_ALL</t>
+  </si>
+  <si>
+    <t>WORKS_BRAND</t>
+  </si>
+  <si>
+    <t>WORKS_MOTION</t>
+  </si>
+  <si>
+    <t>WORKS_INTERFACE</t>
+  </si>
+  <si>
+    <t>WORKS_GRAPHIC</t>
+  </si>
+  <si>
+    <t>WORKS_DIGITAL</t>
+  </si>
+  <si>
+    <t>/works/all</t>
+  </si>
+  <si>
+    <t>/works/brand</t>
+  </si>
+  <si>
+    <t>/works/motion</t>
+  </si>
+  <si>
+    <t>/works/interface</t>
+  </si>
+  <si>
+    <t>/works/graphic</t>
+  </si>
+  <si>
+    <t>/works/digital</t>
   </si>
 </sst>
 </file>
@@ -929,15 +992,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D3DE679-ED2A-44CB-BC3C-25BEAEDDE16B}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1029,6 +1093,54 @@
       </c>
       <c r="B12" s="9" t="s">
         <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>112</v>
+      </c>
+      <c r="B14" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>113</v>
+      </c>
+      <c r="B15" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B16" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>115</v>
+      </c>
+      <c r="B17" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>116</v>
+      </c>
+      <c r="B18" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>117</v>
+      </c>
+      <c r="B19" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1218,7 +1330,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -1385,10 +1497,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1449,6 +1561,54 @@
         <v>85</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B13" t="s">
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
+ Home section 3
</commit_message>
<xml_diff>
--- a/data/text.xlsx
+++ b/data/text.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\ReactJS\_neko_website\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC96701-BB55-48FD-82E1-35C492074E7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EF73F50-5AE2-473B-99E4-27FF5C102522}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3930" yWindow="3540" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3930" yWindow="3540" windowWidth="21600" windowHeight="11385" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COMMON" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="130">
   <si>
     <t>::ID::</t>
   </si>
@@ -499,6 +499,142 @@
   </si>
   <si>
     <t>/works/digital</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;span className='{{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>custom</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>}}'&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFF26A65"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>++</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">&lt;/span&gt;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>projects</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;span className='{{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>custom</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>}}'&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFF26A65"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>++</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">&lt;/span&gt;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dự án</t>
+    </r>
+  </si>
+  <si>
+    <t>SECTION_3_TEXT_1</t>
+  </si>
+  <si>
+    <t>SECTION_3_TEXT_2</t>
+  </si>
+  <si>
+    <t>We built the interest with well-known brands in the market</t>
+  </si>
+  <si>
+    <t>SECTION_3_TEXT_3</t>
   </si>
 </sst>
 </file>
@@ -588,7 +724,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -603,6 +739,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -994,7 +1133,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D3DE679-ED2A-44CB-BC3C-25BEAEDDE16B}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -1497,17 +1636,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
     <col min="2" max="2" width="56.28515625" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="47.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1607,6 +1746,33 @@
       </c>
       <c r="B13" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>126</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>127</v>
+      </c>
+      <c r="B16">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>129</v>
+      </c>
+      <c r="B17" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
+ Home case study
</commit_message>
<xml_diff>
--- a/data/text.xlsx
+++ b/data/text.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\ReactJS\_neko_website\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A8BBEEB-2AEF-4D1F-96E7-F9E07838D8F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B599D41-7C60-4954-8F6C-65DDE3A47473}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3930" yWindow="3540" windowWidth="21600" windowHeight="11385" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="162">
   <si>
     <t>::ID::</t>
   </si>
@@ -636,13 +636,109 @@
   <si>
     <t>We built the interest with well-known
 brands in the market</t>
+  </si>
+  <si>
+    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Praesent bibendum, erat nec lobortis finibus, nisl sapien mollis nisi, quis porta eros urna at ipsum. Nulla hendrerit volutpat nibh, ac mollis velit fringilla eu. Donec dictum arcu nec massa pellentesque, nec imperdiet ante efficitur. Nam molestie vitae nisl nec elementum. Sed ornare risus augue, sit amet dignissim nulla iaculis in. Curabitur at imperdiet mi, at rutrum felis. Pellentesque vestibulum cursus rhoncus. Sed vel nisl non tortor dictum elementum sed lobortis risus. Nam placerat lorem eget justo imperdiet, et luctus orci feugiat. Donec in enim metus. Sed pulvinar ullamcorper erat. Etiam non mi vitae magna condimentum vehicula. Fusce nunc est, efficitur eget purus vel, mollis placerat justo. Mauris sed finibus mauris, lacinia fermentum odio. Etiam at efficitur felis.</t>
+  </si>
+  <si>
+    <t>Lorem ipsum - Product Manager</t>
+  </si>
+  <si>
+    <t>03.svg</t>
+  </si>
+  <si>
+    <t>Donec at finibus quam. Quisque euismod quam nunc, at tempus mauris porttitor at. Quisque aliquet sagittis suscipit. Sed dui diam, finibus hendrerit mi sit amet, vulputate rutrum velit. In convallis dictum justo, nec faucibus est congue non. Nullam sed dolor eget elit molestie dapibus. Phasellus vehicula odio et eros ullamcorper faucibus. Aenean purus erat, laoreet vel ornare et, tristique posuere quam. Duis quis mollis risus. Suspendisse odio erat, tempus at volutpat nec, eleifend in orci. Quisque tellus est, blandit in metus quis, consectetur euismod lectus. Aliquam tincidunt venenatis tortor eu laoreet. Pellentesque tincidunt massa mauris, in pellentesque purus faucibus nec. Quisque a quam finibus, efficitur mauris id, molestie magna. Sed pretium dictum sem, vitae euismod turpis ultrices nec. Donec molestie dapibus odio.</t>
+  </si>
+  <si>
+    <t>Donec Finibus - Director</t>
+  </si>
+  <si>
+    <t>Curabitur placerat leo a sapien aliquam, ut rutrum magna dapibus. Fusce ac enim ante. Phasellus tincidunt pretium justo non interdum. In ultrices ante turpis, id dapibus nulla tempus et. Suspendisse ultricies convallis aliquet. Nullam tristique tortor vel est viverra, et tempus lectus auctor. Suspendisse lacinia felis et arcu tincidunt elementum. Aliquam ac ultricies augue. Nullam elementum justo in ipsum rhoncus auctor. Maecenas accumsan vestibulum risus vel molestie. Ut eleifend imperdiet odio a iaculis. Vivamus rhoncus lobortis mi. Aliquam erat volutpat.</t>
+  </si>
+  <si>
+    <t>Curabitur Leo Sapien - Sale Manager</t>
+  </si>
+  <si>
+    <t>SECTION_4_LOGO_1</t>
+  </si>
+  <si>
+    <t>SECTION_4_TEXT_1</t>
+  </si>
+  <si>
+    <t>SECTION_4_TITLE_1</t>
+  </si>
+  <si>
+    <t>SECTION_4_LOGO_2</t>
+  </si>
+  <si>
+    <t>SECTION_4_TEXT_2</t>
+  </si>
+  <si>
+    <t>SECTION_4_TITLE_2</t>
+  </si>
+  <si>
+    <t>SECTION_4_LOGO_3</t>
+  </si>
+  <si>
+    <t>SECTION_4_TEXT_3</t>
+  </si>
+  <si>
+    <t>SECTION_4_TITLE_3</t>
+  </si>
+  <si>
+    <t>SECTION_4_LOGO_4</t>
+  </si>
+  <si>
+    <t>SECTION_4_TEXT_4</t>
+  </si>
+  <si>
+    <t>SECTION_4_TITLE_4</t>
+  </si>
+  <si>
+    <t>SECTION_4_LOGO_5</t>
+  </si>
+  <si>
+    <t>SECTION_4_TEXT_5</t>
+  </si>
+  <si>
+    <t>SECTION_4_TITLE_5</t>
+  </si>
+  <si>
+    <t>Suspendisse fringilla posuere sem nec accumsan. Pellentesque sapien dolor, egestas a blandit vitae, finibus in tellus. Cras pharetra lorem nec urna sagittis convallis. Sed eu cursus lacus, id ullamcorper nisl. Maecenas finibus aliquam nisi eget finibus. Morbi aliquam id sapien eu tempor. Quisque turpis nisi, aliquam cursus dictum fringilla, cursus cursus quam. Nunc at euismod eros. Vestibulum ante ipsum primis in faucibus orci luctus et ultrices posuere cubilia curae;</t>
+  </si>
+  <si>
+    <t>In iaculis justo a dui scelerisque ultrices ac quis purus. Vivamus maximus libero at imperdiet feugiat. Vestibulum vehicula sem magna, eget pellentesque felis fermentum in. Interdum et malesuada fames ac ante ipsum primis in faucibus. Sed felis diam, bibendum pharetra libero vel, congue fermentum velit. Nullam orci quam, dictum at nisi at, congue finibus metus. Nam tincidunt lorem lacus, non varius est mollis non. Vivamus et pellentesque magna, et ultricies enim. Phasellus augue sem, varius at nunc at, laoreet volutpat turpis. Pellentesque tincidunt dui faucibus lectus interdum, et interdum magna gravida. Integer pretium, eros ut auctor tincidunt, arcu massa maximus libero, non iaculis erat purus congue sem. Fusce quis efficitur dui, a euismod elit. Quisque ex ante, vestibulum sed ex a, maximus scelerisque arcu. In enim sapien, vulputate in risus vitae, auctor sagittis odio. Fusce dictum malesuada sem id volutpat. Donec ac fermentum leo.</t>
+  </si>
+  <si>
+    <t>Suspendisse Fringilla - CEO</t>
+  </si>
+  <si>
+    <t>Iaculis - Lead Developer</t>
+  </si>
+  <si>
+    <t>SECTION_4_BUTTON_1</t>
+  </si>
+  <si>
+    <t>Read case study</t>
+  </si>
+  <si>
+    <t>07.svg</t>
+  </si>
+  <si>
+    <t>06.svg</t>
+  </si>
+  <si>
+    <t>08.svg</t>
+  </si>
+  <si>
+    <t>09.svg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -697,6 +793,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -725,7 +827,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -741,6 +843,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1637,10 +1745,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1776,6 +1884,134 @@
         <v>129</v>
       </c>
     </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>137</v>
+      </c>
+      <c r="B19" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>138</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>139</v>
+      </c>
+      <c r="B21" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>140</v>
+      </c>
+      <c r="B23" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="264" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>141</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>142</v>
+      </c>
+      <c r="B25" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>143</v>
+      </c>
+      <c r="B27" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="181.5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>144</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>145</v>
+      </c>
+      <c r="B29" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>146</v>
+      </c>
+      <c r="B31" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="165" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>147</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>148</v>
+      </c>
+      <c r="B33" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>149</v>
+      </c>
+      <c r="B35" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="313.5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>150</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>151</v>
+      </c>
+      <c r="B37" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>156</v>
+      </c>
+      <c r="B39" t="s">
+        <v>157</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- display case study index
</commit_message>
<xml_diff>
--- a/data/text.xlsx
+++ b/data/text.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\ReactJS\_neko_website\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B599D41-7C60-4954-8F6C-65DDE3A47473}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD2DD80-607C-4B03-A64E-682AE541A8A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3930" yWindow="3540" windowWidth="21600" windowHeight="11385" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="163">
   <si>
     <t>::ID::</t>
   </si>
@@ -631,9 +631,6 @@
     <t>SECTION_3_TEXT_2</t>
   </si>
   <si>
-    <t>SECTION_3_TEXT_3</t>
-  </si>
-  <si>
     <t>We built the interest with well-known
 brands in the market</t>
   </si>
@@ -732,6 +729,12 @@
   </si>
   <si>
     <t>09.svg</t>
+  </si>
+  <si>
+    <t>SECTION_3_PROJECTS_NUM</t>
+  </si>
+  <si>
+    <t>SECTION_4_CASE_STUDY_NUM</t>
   </si>
 </sst>
 </file>
@@ -800,7 +803,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -810,6 +813,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -827,7 +836,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -851,6 +860,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1745,15 +1755,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="1" max="1" width="31.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="56.28515625" customWidth="1"/>
     <col min="3" max="3" width="47.7109375" customWidth="1"/>
   </cols>
@@ -1857,159 +1867,167 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>161</v>
+      </c>
+      <c r="B15" s="13">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>126</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B16" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C16" s="10" t="s">
         <v>125</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>127</v>
-      </c>
-      <c r="B16">
-        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>127</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>128</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>137</v>
-      </c>
-      <c r="B19" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="225" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>138</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>130</v>
+        <v>162</v>
+      </c>
+      <c r="B19" s="13">
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B21" t="s">
         <v>131</v>
       </c>
     </row>
+    <row r="22" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>137</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>129</v>
+      </c>
+    </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B23" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="264" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>141</v>
-      </c>
-      <c r="B24" s="12" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B25" t="s">
-        <v>134</v>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="264" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>140</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B27" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="181.5" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>144</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B29" t="s">
-        <v>136</v>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="181.5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>143</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B31" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="165" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>147</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B33" t="s">
-        <v>154</v>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="165" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>146</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B35" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="313.5" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>150</v>
-      </c>
-      <c r="B36" s="12" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B37" t="s">
-        <v>155</v>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="313.5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>149</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>150</v>
+      </c>
+      <c r="B39" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>155</v>
+      </c>
+      <c r="B41" t="s">
         <v>156</v>
-      </c>
-      <c r="B39" t="s">
-        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* change image background
</commit_message>
<xml_diff>
--- a/data/text.xlsx
+++ b/data/text.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\ReactJS\_neko_website\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E72EF48D-1727-4387-92C3-CFD06C22A834}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A086CDA2-11BD-40CB-8E0B-9CCA33DF0FC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="2730" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COMMON" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="287">
   <si>
     <t>::ID::</t>
   </si>
@@ -1042,24 +1042,6 @@
     <t>/images/blog/blog03.jpg</t>
   </si>
   <si>
-    <t>WORK_1</t>
-  </si>
-  <si>
-    <t>WORK_2</t>
-  </si>
-  <si>
-    <t>WORK_3</t>
-  </si>
-  <si>
-    <t>WORK_4</t>
-  </si>
-  <si>
-    <t>WORK_5</t>
-  </si>
-  <si>
-    <t>/images/work/</t>
-  </si>
-  <si>
     <t>IMAGE::BLOG_1</t>
   </si>
   <si>
@@ -1067,6 +1049,66 @@
   </si>
   <si>
     <t>IMAGE::BLOG_3</t>
+  </si>
+  <si>
+    <t>/images/work/specialized_branding.jpg</t>
+  </si>
+  <si>
+    <t>/images/work/specialized_motion.jpg</t>
+  </si>
+  <si>
+    <t>/images/work/specialized_ui.jpg</t>
+  </si>
+  <si>
+    <t>/images/work/specialized_2D.jpg</t>
+  </si>
+  <si>
+    <t>/images/work/specialized_digital.jpg</t>
+  </si>
+  <si>
+    <t>WORK_SPECIALIZED_1</t>
+  </si>
+  <si>
+    <t>WORK_SPECIALIZED_2</t>
+  </si>
+  <si>
+    <t>WORK_SPECIALIZED_3</t>
+  </si>
+  <si>
+    <t>WORK_SPECIALIZED_4</t>
+  </si>
+  <si>
+    <t>WORK_SPECIALIZED_5</t>
+  </si>
+  <si>
+    <t>SECTION_2_MENU_BG_1</t>
+  </si>
+  <si>
+    <t>SECTION_2_MENU_BG_2</t>
+  </si>
+  <si>
+    <t>SECTION_2_MENU_BG_3</t>
+  </si>
+  <si>
+    <t>SECTION_2_MENU_BG_4</t>
+  </si>
+  <si>
+    <t>SECTION_2_MENU_BG_5</t>
+  </si>
+  <si>
+    <t>rgb(255, 200, 193)</t>
+  </si>
+  <si>
+    <t>rgb(229, 223, 249)</t>
+  </si>
+  <si>
+    <t>rgb(212, 228, 254)</t>
+  </si>
+  <si>
+    <t>rgb(247, 229, 191)</t>
+  </si>
+  <si>
+    <t>rgb(195, 227, 224)</t>
   </si>
 </sst>
 </file>
@@ -1593,8 +1635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D3DE679-ED2A-44CB-BC3C-25BEAEDDE16B}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1798,12 +1840,12 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.5703125" customWidth="1"/>
     <col min="3" max="3" width="18.140625" customWidth="1"/>
   </cols>
@@ -2045,23 +2087,23 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>264</v>
+        <v>272</v>
       </c>
       <c r="B33" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>265</v>
+        <v>273</v>
       </c>
       <c r="B34" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>266</v>
+        <v>274</v>
       </c>
       <c r="B35" t="s">
         <v>269</v>
@@ -2069,18 +2111,18 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>267</v>
+        <v>275</v>
       </c>
       <c r="B36" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>268</v>
+        <v>276</v>
       </c>
       <c r="B37" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -2433,10 +2475,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C52"/>
+  <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A64" sqref="A54:B64"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2521,270 +2563,310 @@
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>105</v>
-      </c>
-      <c r="B11" t="s">
-        <v>110</v>
-      </c>
-    </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B13" t="s">
-        <v>111</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B14" t="s">
-        <v>63</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>108</v>
+      </c>
+      <c r="B15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>109</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>156</v>
-      </c>
-      <c r="B17" s="13">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>126</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>277</v>
+      </c>
+      <c r="B18" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>127</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>128</v>
+        <v>278</v>
+      </c>
+      <c r="B19" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>279</v>
+      </c>
+      <c r="B20" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>157</v>
-      </c>
-      <c r="B21" s="13">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>135</v>
-      </c>
-      <c r="B23" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="225" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+      <c r="B21" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>281</v>
+      </c>
+      <c r="B22" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>136</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+      <c r="B24" s="13">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>137</v>
-      </c>
-      <c r="B25" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>162</v>
-      </c>
-      <c r="B26" t="s">
-        <v>163</v>
+        <v>127</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>138</v>
-      </c>
-      <c r="B28" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="264" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>139</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>131</v>
+        <v>157</v>
+      </c>
+      <c r="B28" s="13">
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B30" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="225" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>164</v>
-      </c>
-      <c r="B31" t="s">
-        <v>165</v>
+        <v>136</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>137</v>
+      </c>
+      <c r="B32" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>141</v>
+        <v>162</v>
       </c>
       <c r="B33" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="181.5" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>142</v>
-      </c>
-      <c r="B34" s="12" t="s">
-        <v>133</v>
+        <v>163</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B35" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="264" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>166</v>
-      </c>
-      <c r="B36" t="s">
-        <v>167</v>
+        <v>139</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>140</v>
+      </c>
+      <c r="B37" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>144</v>
+        <v>164</v>
       </c>
       <c r="B38" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="165" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>145</v>
-      </c>
-      <c r="B39" s="12" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B40" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="181.5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>168</v>
-      </c>
-      <c r="B41" t="s">
-        <v>169</v>
+        <v>142</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>143</v>
+      </c>
+      <c r="B42" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>147</v>
+        <v>166</v>
       </c>
       <c r="B43" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="313.5" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>148</v>
-      </c>
-      <c r="B44" s="12" t="s">
-        <v>151</v>
+        <v>167</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B45" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="165" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>171</v>
-      </c>
-      <c r="B46" t="s">
-        <v>170</v>
+        <v>145</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>146</v>
+      </c>
+      <c r="B47" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
       <c r="B48" t="s">
-        <v>155</v>
+        <v>169</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>182</v>
+        <v>147</v>
       </c>
       <c r="B50" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="313.5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>184</v>
-      </c>
-      <c r="B51" t="s">
-        <v>185</v>
+        <v>148</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>149</v>
+      </c>
+      <c r="B52" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>171</v>
+      </c>
+      <c r="B53" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>154</v>
+      </c>
+      <c r="B55" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>182</v>
+      </c>
+      <c r="B57" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>184</v>
+      </c>
+      <c r="B58" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>186</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B59" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2799,7 +2881,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58674EB5-127B-4328-8233-CC4ED0071AED}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -2825,7 +2907,7 @@
         <v>247</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2853,7 +2935,7 @@
         <v>250</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2881,7 +2963,7 @@
         <v>253</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
- animation blog image
</commit_message>
<xml_diff>
--- a/data/text.xlsx
+++ b/data/text.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\ReactJS\_neko_website\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A086CDA2-11BD-40CB-8E0B-9CCA33DF0FC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED52268-4EAB-4B16-AB65-F6D60F8C39BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="2730" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="2730" windowWidth="21600" windowHeight="11385" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COMMON" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="300">
   <si>
     <t>::ID::</t>
   </si>
@@ -1109,6 +1109,45 @@
   </si>
   <si>
     <t>rgb(195, 227, 224)</t>
+  </si>
+  <si>
+    <t>/blog/1</t>
+  </si>
+  <si>
+    <t>BLOG_4</t>
+  </si>
+  <si>
+    <t>BLOG_5</t>
+  </si>
+  <si>
+    <t>/blog/2</t>
+  </si>
+  <si>
+    <t>/blog/3</t>
+  </si>
+  <si>
+    <t>/blog/4</t>
+  </si>
+  <si>
+    <t>/blog/5</t>
+  </si>
+  <si>
+    <t>LINK_1</t>
+  </si>
+  <si>
+    <t>LINK::BLOG_1</t>
+  </si>
+  <si>
+    <t>LINK_2</t>
+  </si>
+  <si>
+    <t>LINK::BLOG_2</t>
+  </si>
+  <si>
+    <t>LINK_3</t>
+  </si>
+  <si>
+    <t>LINK::BLOG_3</t>
   </si>
 </sst>
 </file>
@@ -1633,10 +1672,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D3DE679-ED2A-44CB-BC3C-25BEAEDDE16B}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27:B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1822,6 +1861,46 @@
       </c>
       <c r="B25" t="s">
         <v>181</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>258</v>
+      </c>
+      <c r="B27" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>259</v>
+      </c>
+      <c r="B28" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>260</v>
+      </c>
+      <c r="B29" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>288</v>
+      </c>
+      <c r="B30" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>289</v>
+      </c>
+      <c r="B31" t="s">
+        <v>293</v>
       </c>
     </row>
   </sheetData>
@@ -2477,7 +2556,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -2879,10 +2958,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58674EB5-127B-4328-8233-CC4ED0071AED}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2927,59 +3006,83 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="6"/>
+      <c r="A5" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>250</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>265</v>
-      </c>
+      <c r="A6" s="14"/>
+      <c r="B6" s="6"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
+        <v>250</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
         <v>251</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B8" s="16" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+    <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
         <v>252</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B9" s="6" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+      <c r="B11" s="6"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
         <v>253</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B12" s="14" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
         <v>254</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B13" s="16" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B14" s="6" t="s">
         <v>191</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
+ Home section 6
</commit_message>
<xml_diff>
--- a/data/text.xlsx
+++ b/data/text.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\ReactJS\_neko_website\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10CBDA37-2665-498A-8C90-48BDB9C34A33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797EBDAB-5F40-4B83-8EAB-B9A382DEE925}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="341">
   <si>
     <t>::ID::</t>
   </si>
@@ -1263,6 +1263,40 @@
   <si>
     <t>Big idea to create your
 brand personality</t>
+  </si>
+  <si>
+    <t>SECTION_6_TEXT_1</t>
+  </si>
+  <si>
+    <t>hmmm…</t>
+  </si>
+  <si>
+    <t>SECTION_6_TEXT_2</t>
+  </si>
+  <si>
+    <t>SECTION_6_TEXT_3</t>
+  </si>
+  <si>
+    <t>Hello, Neko.
+Tell me what you can do!</t>
+  </si>
+  <si>
+    <t>SECTION_6_TEXT_4</t>
+  </si>
+  <si>
+    <t>SECTION_6_TEXT_5</t>
+  </si>
+  <si>
+    <t>Hey Neko. Surprised me!</t>
+  </si>
+  <si>
+    <t>let's
+see</t>
+  </si>
+  <si>
+    <t>Hi, Neko.
+I have many ideas. But I don't know
+where to start...</t>
   </si>
 </sst>
 </file>
@@ -2694,10 +2728,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C59"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3087,6 +3121,46 @@
       </c>
       <c r="B59" t="s">
         <v>185</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>331</v>
+      </c>
+      <c r="B61" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>333</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>334</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>336</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>337</v>
+      </c>
+      <c r="B65" t="s">
+        <v>338</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* CSS grid title
</commit_message>
<xml_diff>
--- a/data/text.xlsx
+++ b/data/text.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\ReactJS\_neko_website\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB9923F5-B0CD-48A2-92B0-55262E10B2C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA577A57-9021-40EA-A2E9-B90D701E2707}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COMMON" sheetId="1" r:id="rId1"/>
@@ -236,121 +236,61 @@
     <t>WORKS_DETAIL_1</t>
   </si>
   <si>
-    <t>/works_detail/1</t>
-  </si>
-  <si>
     <t>WORKS_DETAIL_2</t>
   </si>
   <si>
-    <t>/works_detail/2</t>
-  </si>
-  <si>
     <t>WORKS_DETAIL_3</t>
   </si>
   <si>
-    <t>/works_detail/3</t>
-  </si>
-  <si>
     <t>WORKS_DETAIL_4</t>
   </si>
   <si>
-    <t>/works_detail/4</t>
-  </si>
-  <si>
     <t>WORKS_DETAIL_5</t>
   </si>
   <si>
-    <t>/works_detail/5</t>
-  </si>
-  <si>
     <t>WORKS_DETAIL_6</t>
   </si>
   <si>
-    <t>/works_detail/6</t>
-  </si>
-  <si>
     <t>WORKS_DETAIL_7</t>
   </si>
   <si>
-    <t>/works_detail/7</t>
-  </si>
-  <si>
     <t>WORKS_DETAIL_8</t>
   </si>
   <si>
-    <t>/works_detail/8</t>
-  </si>
-  <si>
     <t>WORKS_DETAIL_9</t>
   </si>
   <si>
-    <t>/works_detail/9</t>
-  </si>
-  <si>
     <t>WORKS_DETAIL_10</t>
   </si>
   <si>
-    <t>/works_detail/10</t>
-  </si>
-  <si>
     <t>WORKS_DETAIL_11</t>
   </si>
   <si>
-    <t>/works_detail/11</t>
-  </si>
-  <si>
     <t>WORKS_DETAIL_12</t>
   </si>
   <si>
-    <t>/works_detail/12</t>
-  </si>
-  <si>
     <t>WORKS_DETAIL_13</t>
   </si>
   <si>
-    <t>/works_detail/13</t>
-  </si>
-  <si>
     <t>WORKS_DETAIL_14</t>
   </si>
   <si>
-    <t>/works_detail/14</t>
-  </si>
-  <si>
     <t>WORKS_DETAIL_15</t>
   </si>
   <si>
-    <t>/works_detail/15</t>
-  </si>
-  <si>
     <t>WORKS_DETAIL_16</t>
   </si>
   <si>
-    <t>/works_detail/16</t>
-  </si>
-  <si>
     <t>WORKS_DETAIL_17</t>
   </si>
   <si>
-    <t>/works_detail/17</t>
-  </si>
-  <si>
     <t>WORKS_DETAIL_18</t>
   </si>
   <si>
-    <t>/works_detail/18</t>
-  </si>
-  <si>
     <t>WORKS_DETAIL_19</t>
   </si>
   <si>
-    <t>/works_detail/19</t>
-  </si>
-  <si>
     <t>WORKS_DETAIL_20</t>
-  </si>
-  <si>
-    <t>/works_detail/20</t>
   </si>
   <si>
     <t>LOGO_1</t>
@@ -2004,6 +1944,66 @@
       </rPr>
       <t>&gt;</t>
     </r>
+  </si>
+  <si>
+    <t>/works/detail/1</t>
+  </si>
+  <si>
+    <t>/works/detail/2</t>
+  </si>
+  <si>
+    <t>/works/detail/3</t>
+  </si>
+  <si>
+    <t>/works/detail/4</t>
+  </si>
+  <si>
+    <t>/works/detail/5</t>
+  </si>
+  <si>
+    <t>/works/detail/6</t>
+  </si>
+  <si>
+    <t>/works/detail/7</t>
+  </si>
+  <si>
+    <t>/works/detail/8</t>
+  </si>
+  <si>
+    <t>/works/detail/9</t>
+  </si>
+  <si>
+    <t>/works/detail/10</t>
+  </si>
+  <si>
+    <t>/works/detail/11</t>
+  </si>
+  <si>
+    <t>/works/detail/12</t>
+  </si>
+  <si>
+    <t>/works/detail/13</t>
+  </si>
+  <si>
+    <t>/works/detail/14</t>
+  </si>
+  <si>
+    <t>/works/detail/15</t>
+  </si>
+  <si>
+    <t>/works/detail/16</t>
+  </si>
+  <si>
+    <t>/works/detail/17</t>
+  </si>
+  <si>
+    <t>/works/detail/18</t>
+  </si>
+  <si>
+    <t>/works/detail/19</t>
+  </si>
+  <si>
+    <t>/works/detail/20</t>
   </si>
 </sst>
 </file>
@@ -2649,8 +2649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2785,10 +2785,10 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>225</v>
+        <v>205</v>
       </c>
       <c r="B18" t="s">
-        <v>545</v>
+        <v>525</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2804,7 +2804,7 @@
         <v>43</v>
       </c>
       <c r="B20" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -2900,159 +2900,159 @@
         <v>66</v>
       </c>
       <c r="B35" t="s">
-        <v>67</v>
+        <v>532</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B36" t="s">
-        <v>69</v>
+        <v>533</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B37" t="s">
-        <v>71</v>
+        <v>534</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B38" t="s">
-        <v>73</v>
+        <v>535</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B39" t="s">
-        <v>75</v>
+        <v>536</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B40" t="s">
-        <v>77</v>
+        <v>537</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B41" t="s">
-        <v>79</v>
+        <v>538</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B42" t="s">
-        <v>81</v>
+        <v>539</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B43" t="s">
-        <v>83</v>
+        <v>540</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B44" t="s">
-        <v>85</v>
+        <v>541</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B45" t="s">
-        <v>87</v>
+        <v>542</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B46" t="s">
-        <v>89</v>
+        <v>543</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B47" t="s">
-        <v>91</v>
+        <v>544</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="B48" t="s">
-        <v>93</v>
+        <v>545</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="B49" t="s">
-        <v>95</v>
+        <v>546</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="B50" t="s">
-        <v>97</v>
+        <v>547</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="B51" t="s">
-        <v>99</v>
+        <v>548</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="B52" t="s">
-        <v>101</v>
+        <v>549</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="B53" t="s">
-        <v>103</v>
+        <v>550</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="B54" t="s">
-        <v>105</v>
+        <v>551</v>
       </c>
     </row>
   </sheetData>
@@ -3095,162 +3095,162 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="B4" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="B5" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="B6" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="B7" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="B8" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="B9" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="B10" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="B11" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="B12" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="B13" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="B14" t="s">
-        <v>131</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="B15" t="s">
-        <v>133</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
       <c r="B16" t="s">
-        <v>135</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
       <c r="B17" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="B18" t="s">
-        <v>139</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="B19" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>142</v>
+        <v>122</v>
       </c>
       <c r="B20" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
       <c r="B21" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -3258,7 +3258,7 @@
         <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -3266,63 +3266,63 @@
         <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
       <c r="B26" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="B28" t="s">
-        <v>151</v>
+        <v>131</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>152</v>
+        <v>132</v>
       </c>
       <c r="B29" t="s">
-        <v>153</v>
+        <v>133</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>154</v>
+        <v>134</v>
       </c>
       <c r="B30" t="s">
-        <v>155</v>
+        <v>135</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>156</v>
+        <v>136</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>157</v>
+        <v>137</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>158</v>
+        <v>138</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>159</v>
+        <v>139</v>
       </c>
     </row>
     <row r="33" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -3330,7 +3330,7 @@
         <v>56</v>
       </c>
       <c r="B35" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -3338,7 +3338,7 @@
         <v>58</v>
       </c>
       <c r="B36" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -3346,47 +3346,47 @@
         <v>60</v>
       </c>
       <c r="B37" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="B39" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
       <c r="B40" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="B41" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
       <c r="B42" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="B43" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -3394,159 +3394,159 @@
         <v>66</v>
       </c>
       <c r="B45" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B46" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B47" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B48" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B49" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B50" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B51" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B52" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B53" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B54" t="s">
-        <v>184</v>
+        <v>164</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B55" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B56" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B57" t="s">
-        <v>187</v>
+        <v>167</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="B58" t="s">
-        <v>188</v>
+        <v>168</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="B59" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="B60" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="B61" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="B62" t="s">
-        <v>192</v>
+        <v>172</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="B63" t="s">
-        <v>193</v>
+        <v>173</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="B64" t="s">
-        <v>194</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -3584,13 +3584,13 @@
     </row>
     <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3601,7 +3601,7 @@
         <v>15</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3609,10 +3609,10 @@
         <v>17</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3623,7 +3623,7 @@
         <v>19</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3634,7 +3634,7 @@
         <v>21</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -3654,7 +3654,7 @@
         <v>25</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -3664,68 +3664,68 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>205</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>206</v>
+        <v>186</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>209</v>
+        <v>189</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>213</v>
+        <v>193</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>214</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>215</v>
+        <v>195</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>216</v>
+        <v>196</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>217</v>
+        <v>197</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>218</v>
+        <v>198</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>219</v>
+        <v>199</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>220</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -3733,7 +3733,7 @@
         <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>221</v>
+        <v>201</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -3741,7 +3741,7 @@
         <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -3749,7 +3749,7 @@
         <v>37</v>
       </c>
       <c r="B19" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -3757,15 +3757,15 @@
         <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>224</v>
+        <v>204</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>225</v>
+        <v>205</v>
       </c>
       <c r="B21" t="s">
-        <v>226</v>
+        <v>206</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -3773,47 +3773,47 @@
         <v>41</v>
       </c>
       <c r="B22" t="s">
-        <v>227</v>
+        <v>207</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>546</v>
+        <v>526</v>
       </c>
       <c r="B24" t="s">
-        <v>276</v>
+        <v>256</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>547</v>
+        <v>527</v>
       </c>
       <c r="B25" t="s">
-        <v>277</v>
+        <v>257</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>548</v>
+        <v>528</v>
       </c>
       <c r="B26" t="s">
-        <v>278</v>
+        <v>258</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>549</v>
+        <v>529</v>
       </c>
       <c r="B27" t="s">
-        <v>279</v>
+        <v>259</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>550</v>
+        <v>530</v>
       </c>
       <c r="B28" t="s">
-        <v>280</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -3850,138 +3850,138 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="B2" t="s">
-        <v>229</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="B3" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="B5" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>234</v>
+        <v>214</v>
       </c>
       <c r="B7" t="s">
-        <v>235</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
       <c r="B8" t="s">
-        <v>237</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>238</v>
+        <v>218</v>
       </c>
       <c r="B9" t="s">
-        <v>239</v>
+        <v>219</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="B11" t="s">
-        <v>241</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>242</v>
+        <v>222</v>
       </c>
       <c r="B12" t="s">
-        <v>243</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="B13" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>245</v>
+        <v>225</v>
       </c>
       <c r="B14" t="s">
-        <v>246</v>
+        <v>226</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>247</v>
+        <v>227</v>
       </c>
       <c r="B15" t="s">
-        <v>248</v>
+        <v>228</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>249</v>
+        <v>229</v>
       </c>
       <c r="B16" t="s">
-        <v>227</v>
+        <v>207</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>250</v>
+        <v>230</v>
       </c>
       <c r="B18" t="s">
-        <v>251</v>
+        <v>231</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>252</v>
+        <v>232</v>
       </c>
       <c r="B19" t="s">
-        <v>253</v>
+        <v>233</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>254</v>
+        <v>234</v>
       </c>
       <c r="B20" t="s">
-        <v>255</v>
+        <v>235</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>256</v>
+        <v>236</v>
       </c>
       <c r="B21" t="s">
-        <v>257</v>
+        <v>237</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>258</v>
+        <v>238</v>
       </c>
       <c r="B23" t="s">
-        <v>259</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -4019,71 +4019,71 @@
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>260</v>
+        <v>240</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>261</v>
+        <v>241</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>262</v>
+        <v>242</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>264</v>
+        <v>244</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>265</v>
+        <v>245</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>266</v>
+        <v>246</v>
       </c>
       <c r="B5" t="s">
-        <v>267</v>
+        <v>247</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>268</v>
+        <v>248</v>
       </c>
       <c r="B6" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="B7" t="s">
-        <v>271</v>
+        <v>251</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>272</v>
+        <v>252</v>
       </c>
       <c r="B8" t="s">
-        <v>273</v>
+        <v>253</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>274</v>
+        <v>254</v>
       </c>
       <c r="B10" t="s">
-        <v>275</v>
+        <v>255</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>281</v>
+        <v>261</v>
       </c>
       <c r="B12" s="11">
         <v>85</v>
@@ -4091,26 +4091,26 @@
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>282</v>
+        <v>262</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>283</v>
+        <v>263</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>284</v>
+        <v>264</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>285</v>
+        <v>265</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>286</v>
+        <v>266</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>287</v>
+        <v>267</v>
       </c>
       <c r="B16" s="11">
         <v>5</v>
@@ -4118,234 +4118,234 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>288</v>
+        <v>268</v>
       </c>
       <c r="B18" t="s">
-        <v>289</v>
+        <v>269</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>290</v>
+        <v>270</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>291</v>
+        <v>271</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>292</v>
+        <v>272</v>
       </c>
       <c r="B20" t="s">
-        <v>293</v>
+        <v>273</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>294</v>
+        <v>274</v>
       </c>
       <c r="B21" t="s">
-        <v>295</v>
+        <v>275</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>296</v>
+        <v>276</v>
       </c>
       <c r="B23" t="s">
-        <v>297</v>
+        <v>277</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="264" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>298</v>
+        <v>278</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>299</v>
+        <v>279</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>300</v>
+        <v>280</v>
       </c>
       <c r="B25" t="s">
-        <v>301</v>
+        <v>281</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>302</v>
+        <v>282</v>
       </c>
       <c r="B26" t="s">
-        <v>303</v>
+        <v>283</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>304</v>
+        <v>284</v>
       </c>
       <c r="B28" t="s">
-        <v>305</v>
+        <v>285</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="181.5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>306</v>
+        <v>286</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>307</v>
+        <v>287</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>308</v>
+        <v>288</v>
       </c>
       <c r="B30" t="s">
-        <v>309</v>
+        <v>289</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>310</v>
+        <v>290</v>
       </c>
       <c r="B31" t="s">
-        <v>311</v>
+        <v>291</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>312</v>
+        <v>292</v>
       </c>
       <c r="B33" t="s">
-        <v>313</v>
+        <v>293</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="165" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>314</v>
+        <v>294</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>315</v>
+        <v>295</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>316</v>
+        <v>296</v>
       </c>
       <c r="B35" t="s">
-        <v>317</v>
+        <v>297</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>318</v>
+        <v>298</v>
       </c>
       <c r="B36" t="s">
-        <v>319</v>
+        <v>299</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>320</v>
+        <v>300</v>
       </c>
       <c r="B38" t="s">
-        <v>321</v>
+        <v>301</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="313.5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>322</v>
+        <v>302</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>323</v>
+        <v>303</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>324</v>
+        <v>304</v>
       </c>
       <c r="B40" t="s">
-        <v>325</v>
+        <v>305</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>326</v>
+        <v>306</v>
       </c>
       <c r="B41" t="s">
-        <v>327</v>
+        <v>307</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>328</v>
+        <v>308</v>
       </c>
       <c r="B43" t="s">
-        <v>329</v>
+        <v>309</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>330</v>
+        <v>310</v>
       </c>
       <c r="B45" t="s">
-        <v>331</v>
+        <v>311</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>332</v>
+        <v>312</v>
       </c>
       <c r="B46" t="s">
-        <v>333</v>
+        <v>313</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>334</v>
+        <v>314</v>
       </c>
       <c r="B47" t="s">
-        <v>335</v>
+        <v>315</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>336</v>
+        <v>316</v>
       </c>
       <c r="B49" t="s">
-        <v>337</v>
+        <v>317</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>338</v>
+        <v>318</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>339</v>
+        <v>319</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>340</v>
+        <v>320</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>341</v>
+        <v>321</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>342</v>
+        <v>322</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>343</v>
+        <v>323</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>344</v>
+        <v>324</v>
       </c>
       <c r="B53" t="s">
-        <v>345</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -4382,42 +4382,42 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>346</v>
+        <v>326</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>347</v>
+        <v>327</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>348</v>
+        <v>328</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>349</v>
+        <v>329</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>350</v>
+        <v>330</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>351</v>
+        <v>331</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="210" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>352</v>
+        <v>332</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>353</v>
+        <v>333</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>354</v>
+        <v>334</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>355</v>
+        <v>335</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -4426,42 +4426,42 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>356</v>
+        <v>336</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>357</v>
+        <v>337</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>358</v>
+        <v>338</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>359</v>
+        <v>339</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>360</v>
+        <v>340</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>361</v>
+        <v>341</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="247.5" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
-        <v>362</v>
+        <v>342</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>363</v>
+        <v>343</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>364</v>
+        <v>344</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>365</v>
+        <v>345</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -4470,42 +4470,42 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>366</v>
+        <v>346</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>367</v>
+        <v>347</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>368</v>
+        <v>348</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>369</v>
+        <v>349</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>370</v>
+        <v>350</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>371</v>
+        <v>351</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="198" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
-        <v>372</v>
+        <v>352</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>373</v>
+        <v>353</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>374</v>
+        <v>354</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>375</v>
+        <v>355</v>
       </c>
     </row>
   </sheetData>
@@ -4542,10 +4542,10 @@
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>260</v>
+        <v>240</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>376</v>
+        <v>356</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -4553,130 +4553,130 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>377</v>
+        <v>357</v>
       </c>
       <c r="B4" t="s">
-        <v>378</v>
+        <v>358</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>379</v>
+        <v>359</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>380</v>
+        <v>360</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>381</v>
+        <v>361</v>
       </c>
       <c r="B6" t="s">
-        <v>382</v>
+        <v>362</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>383</v>
+        <v>363</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>384</v>
+        <v>364</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>385</v>
+        <v>365</v>
       </c>
       <c r="B8" t="s">
-        <v>386</v>
+        <v>366</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>387</v>
+        <v>367</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>388</v>
+        <v>368</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>389</v>
+        <v>369</v>
       </c>
       <c r="B10" t="s">
-        <v>271</v>
+        <v>251</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>390</v>
+        <v>370</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>273</v>
+        <v>253</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>282</v>
+        <v>262</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>391</v>
+        <v>371</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>290</v>
+        <v>270</v>
       </c>
       <c r="B15" t="s">
-        <v>392</v>
+        <v>372</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>298</v>
+        <v>278</v>
       </c>
       <c r="B16" t="s">
-        <v>393</v>
+        <v>373</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>306</v>
+        <v>286</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>394</v>
+        <v>374</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>395</v>
+        <v>375</v>
       </c>
       <c r="B19" t="s">
-        <v>396</v>
+        <v>376</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="B20" t="s">
-        <v>398</v>
+        <v>378</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>399</v>
+        <v>379</v>
       </c>
       <c r="B21" t="s">
-        <v>400</v>
+        <v>380</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>401</v>
+        <v>381</v>
       </c>
       <c r="B22" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -4689,8 +4689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AMK122"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4715,810 +4715,810 @@
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>260</v>
+        <v>240</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>551</v>
+        <v>531</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>346</v>
+        <v>326</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>415</v>
+        <v>395</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>404</v>
+        <v>384</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>405</v>
+        <v>385</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>350</v>
+        <v>330</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>351</v>
+        <v>331</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="150" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>352</v>
+        <v>332</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>353</v>
+        <v>333</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>354</v>
+        <v>334</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>416</v>
+        <v>396</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>356</v>
+        <v>336</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>417</v>
+        <v>397</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
-        <v>406</v>
+        <v>386</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>407</v>
+        <v>387</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>360</v>
+        <v>340</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>361</v>
+        <v>341</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="150" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>362</v>
+        <v>342</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>363</v>
+        <v>343</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>364</v>
+        <v>344</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>418</v>
+        <v>398</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>366</v>
+        <v>346</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>419</v>
+        <v>399</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>408</v>
+        <v>388</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>409</v>
+        <v>389</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>370</v>
+        <v>350</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>371</v>
+        <v>351</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
-        <v>372</v>
+        <v>352</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>373</v>
+        <v>353</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>374</v>
+        <v>354</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>420</v>
+        <v>400</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
-        <v>410</v>
+        <v>390</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>421</v>
+        <v>401</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
-        <v>411</v>
+        <v>391</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>433</v>
+        <v>413</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
-        <v>412</v>
+        <v>392</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>423</v>
+        <v>403</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="247.5" x14ac:dyDescent="0.3">
       <c r="A25" s="18" t="s">
-        <v>413</v>
+        <v>393</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>299</v>
+        <v>279</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
-        <v>414</v>
+        <v>394</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>422</v>
+        <v>402</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
-        <v>424</v>
+        <v>404</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>425</v>
+        <v>405</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
-        <v>426</v>
+        <v>406</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>432</v>
+        <v>412</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
-        <v>427</v>
+        <v>407</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>431</v>
+        <v>411</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="165" x14ac:dyDescent="0.3">
       <c r="A31" s="18" t="s">
-        <v>428</v>
+        <v>408</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>307</v>
+        <v>287</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
-        <v>429</v>
+        <v>409</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>430</v>
+        <v>410</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
-        <v>434</v>
+        <v>414</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>435</v>
+        <v>415</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
-        <v>436</v>
+        <v>416</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>405</v>
+        <v>385</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
-        <v>437</v>
+        <v>417</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>351</v>
+        <v>331</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A37" s="18" t="s">
-        <v>438</v>
+        <v>418</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>353</v>
+        <v>333</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="18" t="s">
-        <v>439</v>
+        <v>419</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>440</v>
+        <v>420</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="18" t="s">
-        <v>441</v>
+        <v>421</v>
       </c>
       <c r="B40" s="18" t="s">
-        <v>442</v>
+        <v>422</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="18" t="s">
-        <v>443</v>
+        <v>423</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>407</v>
+        <v>387</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="18" t="s">
-        <v>444</v>
+        <v>424</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>361</v>
+        <v>341</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A43" s="18" t="s">
-        <v>445</v>
+        <v>425</v>
       </c>
       <c r="B43" s="18" t="s">
-        <v>363</v>
+        <v>343</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="18" t="s">
-        <v>446</v>
+        <v>426</v>
       </c>
       <c r="B44" s="18" t="s">
-        <v>447</v>
+        <v>427</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="18" t="s">
-        <v>448</v>
+        <v>428</v>
       </c>
       <c r="B46" s="18" t="s">
-        <v>449</v>
+        <v>429</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="18" t="s">
-        <v>450</v>
+        <v>430</v>
       </c>
       <c r="B47" s="21" t="s">
-        <v>409</v>
+        <v>389</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="18" t="s">
-        <v>451</v>
+        <v>431</v>
       </c>
       <c r="B48" s="18" t="s">
-        <v>371</v>
+        <v>351</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A49" s="18" t="s">
-        <v>452</v>
+        <v>432</v>
       </c>
       <c r="B49" s="18" t="s">
-        <v>373</v>
+        <v>353</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="18" t="s">
-        <v>453</v>
+        <v>433</v>
       </c>
       <c r="B50" s="18" t="s">
-        <v>454</v>
+        <v>434</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="18" t="s">
-        <v>455</v>
+        <v>435</v>
       </c>
       <c r="B52" s="18" t="s">
-        <v>456</v>
+        <v>436</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="18" t="s">
-        <v>457</v>
+        <v>437</v>
       </c>
       <c r="B53" s="21" t="s">
-        <v>433</v>
+        <v>413</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="18" t="s">
-        <v>458</v>
+        <v>438</v>
       </c>
       <c r="B54" s="18" t="s">
-        <v>423</v>
+        <v>403</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="247.5" x14ac:dyDescent="0.3">
       <c r="A55" s="18" t="s">
-        <v>459</v>
+        <v>439</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>299</v>
+        <v>279</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="18" t="s">
-        <v>460</v>
+        <v>440</v>
       </c>
       <c r="B56" s="18" t="s">
-        <v>461</v>
+        <v>441</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="18" t="s">
-        <v>462</v>
+        <v>442</v>
       </c>
       <c r="B58" s="18" t="s">
-        <v>463</v>
+        <v>443</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="18" t="s">
-        <v>464</v>
+        <v>444</v>
       </c>
       <c r="B59" s="21" t="s">
-        <v>432</v>
+        <v>412</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="18" t="s">
-        <v>465</v>
+        <v>445</v>
       </c>
       <c r="B60" s="18" t="s">
-        <v>431</v>
+        <v>411</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="165" x14ac:dyDescent="0.3">
       <c r="A61" s="18" t="s">
-        <v>466</v>
+        <v>446</v>
       </c>
       <c r="B61" s="14" t="s">
-        <v>307</v>
+        <v>287</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="18" t="s">
-        <v>467</v>
+        <v>447</v>
       </c>
       <c r="B62" s="18" t="s">
-        <v>468</v>
+        <v>448</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="18" t="s">
-        <v>469</v>
+        <v>449</v>
       </c>
       <c r="B64" s="18" t="s">
-        <v>470</v>
+        <v>450</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="18" t="s">
-        <v>471</v>
+        <v>451</v>
       </c>
       <c r="B65" s="21" t="s">
-        <v>405</v>
+        <v>385</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A66" s="18" t="s">
-        <v>472</v>
+        <v>452</v>
       </c>
       <c r="B66" s="18" t="s">
-        <v>351</v>
+        <v>331</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A67" s="18" t="s">
-        <v>473</v>
+        <v>453</v>
       </c>
       <c r="B67" s="18" t="s">
-        <v>353</v>
+        <v>333</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="18" t="s">
-        <v>474</v>
+        <v>454</v>
       </c>
       <c r="B68" s="18" t="s">
-        <v>475</v>
+        <v>455</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="18" t="s">
-        <v>476</v>
+        <v>456</v>
       </c>
       <c r="B70" s="18" t="s">
-        <v>477</v>
+        <v>457</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="18" t="s">
-        <v>478</v>
+        <v>458</v>
       </c>
       <c r="B71" s="21" t="s">
-        <v>483</v>
+        <v>463</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="18" t="s">
-        <v>479</v>
+        <v>459</v>
       </c>
       <c r="B72" s="18" t="s">
-        <v>361</v>
+        <v>341</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A73" s="18" t="s">
-        <v>480</v>
+        <v>460</v>
       </c>
       <c r="B73" s="18" t="s">
-        <v>363</v>
+        <v>343</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="18" t="s">
-        <v>481</v>
+        <v>461</v>
       </c>
       <c r="B74" s="18" t="s">
-        <v>482</v>
+        <v>462</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="18" t="s">
-        <v>484</v>
+        <v>464</v>
       </c>
       <c r="B76" s="18" t="s">
-        <v>485</v>
+        <v>465</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="18" t="s">
-        <v>486</v>
+        <v>466</v>
       </c>
       <c r="B77" s="21" t="s">
-        <v>487</v>
+        <v>467</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="18" t="s">
-        <v>488</v>
+        <v>468</v>
       </c>
       <c r="B78" s="18" t="s">
-        <v>371</v>
+        <v>351</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A79" s="18" t="s">
-        <v>489</v>
+        <v>469</v>
       </c>
       <c r="B79" s="18" t="s">
-        <v>373</v>
+        <v>353</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="18" t="s">
-        <v>490</v>
+        <v>470</v>
       </c>
       <c r="B80" s="18" t="s">
-        <v>491</v>
+        <v>471</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="18" t="s">
-        <v>492</v>
+        <v>472</v>
       </c>
       <c r="B82" s="18" t="s">
-        <v>493</v>
+        <v>473</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="18" t="s">
-        <v>494</v>
+        <v>474</v>
       </c>
       <c r="B83" s="21" t="s">
-        <v>495</v>
+        <v>475</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="18" t="s">
-        <v>496</v>
+        <v>476</v>
       </c>
       <c r="B84" s="18" t="s">
-        <v>423</v>
+        <v>403</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="247.5" x14ac:dyDescent="0.3">
       <c r="A85" s="18" t="s">
-        <v>497</v>
+        <v>477</v>
       </c>
       <c r="B85" s="14" t="s">
-        <v>299</v>
+        <v>279</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="18" t="s">
-        <v>498</v>
+        <v>478</v>
       </c>
       <c r="B86" s="18" t="s">
-        <v>499</v>
+        <v>479</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="18" t="s">
-        <v>500</v>
+        <v>480</v>
       </c>
       <c r="B88" s="18" t="s">
-        <v>501</v>
+        <v>481</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="18" t="s">
-        <v>502</v>
+        <v>482</v>
       </c>
       <c r="B89" s="21" t="s">
-        <v>503</v>
+        <v>483</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="18" t="s">
-        <v>504</v>
+        <v>484</v>
       </c>
       <c r="B90" s="18" t="s">
-        <v>431</v>
+        <v>411</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="165" x14ac:dyDescent="0.3">
       <c r="A91" s="18" t="s">
-        <v>505</v>
+        <v>485</v>
       </c>
       <c r="B91" s="14" t="s">
-        <v>307</v>
+        <v>287</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="18" t="s">
-        <v>506</v>
+        <v>486</v>
       </c>
       <c r="B92" s="18" t="s">
-        <v>507</v>
+        <v>487</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="18" t="s">
-        <v>508</v>
+        <v>488</v>
       </c>
       <c r="B94" s="18" t="s">
-        <v>509</v>
+        <v>489</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" s="18" t="s">
-        <v>510</v>
+        <v>490</v>
       </c>
       <c r="B95" s="21" t="s">
-        <v>483</v>
+        <v>463</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A96" s="18" t="s">
-        <v>511</v>
+        <v>491</v>
       </c>
       <c r="B96" s="18" t="s">
-        <v>351</v>
+        <v>331</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A97" s="18" t="s">
-        <v>512</v>
+        <v>492</v>
       </c>
       <c r="B97" s="18" t="s">
-        <v>353</v>
+        <v>333</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="18" t="s">
-        <v>513</v>
+        <v>493</v>
       </c>
       <c r="B98" s="18" t="s">
-        <v>514</v>
+        <v>494</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="18" t="s">
-        <v>515</v>
+        <v>495</v>
       </c>
       <c r="B100" s="18" t="s">
-        <v>516</v>
+        <v>496</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="18" t="s">
-        <v>517</v>
+        <v>497</v>
       </c>
       <c r="B101" s="21" t="s">
-        <v>518</v>
+        <v>498</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" s="18" t="s">
-        <v>519</v>
+        <v>499</v>
       </c>
       <c r="B102" s="18" t="s">
-        <v>361</v>
+        <v>341</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A103" s="18" t="s">
-        <v>520</v>
+        <v>500</v>
       </c>
       <c r="B103" s="18" t="s">
-        <v>363</v>
+        <v>343</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="18" t="s">
-        <v>521</v>
+        <v>501</v>
       </c>
       <c r="B104" s="18" t="s">
-        <v>522</v>
+        <v>502</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="18" t="s">
-        <v>523</v>
+        <v>503</v>
       </c>
       <c r="B106" s="18" t="s">
-        <v>524</v>
+        <v>504</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="18" t="s">
-        <v>525</v>
+        <v>505</v>
       </c>
       <c r="B107" s="21" t="s">
-        <v>526</v>
+        <v>506</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" s="18" t="s">
-        <v>527</v>
+        <v>507</v>
       </c>
       <c r="B108" s="18" t="s">
-        <v>371</v>
+        <v>351</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A109" s="18" t="s">
-        <v>528</v>
+        <v>508</v>
       </c>
       <c r="B109" s="18" t="s">
-        <v>373</v>
+        <v>353</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="18" t="s">
-        <v>529</v>
+        <v>509</v>
       </c>
       <c r="B110" s="18" t="s">
-        <v>530</v>
+        <v>510</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="18" t="s">
-        <v>531</v>
+        <v>511</v>
       </c>
       <c r="B112" s="18" t="s">
-        <v>532</v>
+        <v>512</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="18" t="s">
-        <v>533</v>
+        <v>513</v>
       </c>
       <c r="B113" s="21" t="s">
-        <v>433</v>
+        <v>413</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="18" t="s">
-        <v>534</v>
+        <v>514</v>
       </c>
       <c r="B114" s="18" t="s">
-        <v>423</v>
+        <v>403</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="247.5" x14ac:dyDescent="0.3">
       <c r="A115" s="18" t="s">
-        <v>535</v>
+        <v>515</v>
       </c>
       <c r="B115" s="14" t="s">
-        <v>299</v>
+        <v>279</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="18" t="s">
-        <v>536</v>
+        <v>516</v>
       </c>
       <c r="B116" s="18" t="s">
-        <v>537</v>
+        <v>517</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="18" t="s">
-        <v>538</v>
+        <v>518</v>
       </c>
       <c r="B118" s="18" t="s">
-        <v>539</v>
+        <v>519</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="18" t="s">
-        <v>540</v>
+        <v>520</v>
       </c>
       <c r="B119" s="21" t="s">
-        <v>432</v>
+        <v>412</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A120" s="18" t="s">
-        <v>541</v>
+        <v>521</v>
       </c>
       <c r="B120" s="18" t="s">
-        <v>431</v>
+        <v>411</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="165" x14ac:dyDescent="0.3">
       <c r="A121" s="18" t="s">
-        <v>542</v>
+        <v>522</v>
       </c>
       <c r="B121" s="14" t="s">
-        <v>307</v>
+        <v>287</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="18" t="s">
-        <v>543</v>
+        <v>523</v>
       </c>
       <c r="B122" s="18" t="s">
-        <v>544</v>
+        <v>524</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* hover menu color * bg style
</commit_message>
<xml_diff>
--- a/data/text.xlsx
+++ b/data/text.xlsx
@@ -820,31 +820,31 @@
     <t xml:space="preserve">WORKS_BRAND_BG</t>
   </si>
   <si>
-    <t xml:space="preserve">rgb(255, 200, 193)</t>
+    <t xml:space="preserve">rgb(186, 132, 132)</t>
   </si>
   <si>
     <t xml:space="preserve">WORKS_MOTION_BG</t>
   </si>
   <si>
-    <t xml:space="preserve">rgb(229, 223, 249)</t>
+    <t xml:space="preserve">rgb(213, 207, 233)</t>
   </si>
   <si>
     <t xml:space="preserve">WORKS_INTERFACE_BG</t>
   </si>
   <si>
-    <t xml:space="preserve">rgb(212, 228, 254)</t>
+    <t xml:space="preserve">rgb(165, 181, 206)</t>
   </si>
   <si>
     <t xml:space="preserve">WORKS_GRAPHICS_BG</t>
   </si>
   <si>
-    <t xml:space="preserve">rgb(247, 229, 191)</t>
+    <t xml:space="preserve">rgb(162, 138, 104)</t>
   </si>
   <si>
     <t xml:space="preserve">WORKS_DIGITAL_BG</t>
   </si>
   <si>
-    <t xml:space="preserve">rgb(195, 227, 224)</t>
+    <t xml:space="preserve">Rgb(120, 182, 169)</t>
   </si>
   <si>
     <t xml:space="preserve">SECONDARY_TITLE</t>
@@ -3529,7 +3529,7 @@
   </sheetPr>
   <dimension ref="A1:C81"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H29" activeCellId="0" sqref="H29"/>
     </sheetView>
   </sheetViews>
@@ -4138,8 +4138,8 @@
   </sheetPr>
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4598,7 +4598,7 @@
   </sheetPr>
   <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B56" activeCellId="0" sqref="B56"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
* link to portfolio
</commit_message>
<xml_diff>
--- a/data/text.xlsx
+++ b/data/text.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="COMMON" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="634">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="637">
   <si>
     <t xml:space="preserve">::ID::</t>
   </si>
@@ -709,13 +709,13 @@
     <t xml:space="preserve">/images/capabilities/closeup.png</t>
   </si>
   <si>
+    <t xml:space="preserve">ABOUT_WHAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/images/about/What_we_do.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">ABOUT_WHO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/images/about/What_we_do.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABOUT_WHAT</t>
   </si>
   <si>
     <t xml:space="preserve">/images/about/Who_we_are.png</t>
@@ -978,13 +978,13 @@
     <t xml:space="preserve">SECTION_1_BUTTON_2</t>
   </si>
   <si>
-    <t xml:space="preserve">View all works</t>
+    <t xml:space="preserve">View portfolio</t>
   </si>
   <si>
     <t xml:space="preserve">SECTION_1_BUTTON_2_LINK</t>
   </si>
   <si>
-    <t xml:space="preserve">LINK::WORKS_ALL</t>
+    <t xml:space="preserve">LINK::PORTFOLIO</t>
   </si>
   <si>
     <t xml:space="preserve">SECTION_2_TEXT_1</t>
@@ -2429,6 +2429,15 @@
   </si>
   <si>
     <t xml:space="preserve">LINK::WORKS_DIGITAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUTTON_DEFAULT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">View Portfolio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LINK_DEFAULT</t>
   </si>
 </sst>
 </file>
@@ -2826,10 +2835,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3056,6 +3065,22 @@
       </c>
       <c r="B32" s="10" t="s">
         <v>633</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>634</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>636</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -3529,8 +3554,8 @@
   </sheetPr>
   <dimension ref="A1:C81"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H29" activeCellId="0" sqref="H29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A82" activeCellId="0" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4138,7 +4163,7 @@
   </sheetPr>
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
     </sheetView>
   </sheetViews>
@@ -4599,7 +4624,7 @@
   <dimension ref="A1:C62"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B56" activeCellId="0" sqref="B56"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5201,7 +5226,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5300,7 +5325,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>444</v>
       </c>

</xml_diff>

<commit_message>
+ Contact page + Streamline page
</commit_message>
<xml_diff>
--- a/data/text.xlsx
+++ b/data/text.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="COMMON" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,6 +18,8 @@
     <sheet name="ABOUT" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="WORKS" sheetId="9" state="visible" r:id="rId10"/>
     <sheet name="CAPABILITIES" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="CONTACT" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="STREAMLINE" sheetId="12" state="visible" r:id="rId13"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="639">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="641">
   <si>
     <t xml:space="preserve">::ID::</t>
   </si>
@@ -2511,6 +2513,120 @@
   </si>
   <si>
     <t xml:space="preserve">LINK_DEFAULT</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;span className='{{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF70AD47"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">custom</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">}}'&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFED7D31"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">One mail</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;/span&gt;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">can solve them all!</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;span className='{{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF70AD47"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">custom</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">}}'&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFED7D31"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Streamline</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;/span&gt;</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2666,7 +2782,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2721,14 +2837,6 @@
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -2831,14 +2939,14 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.71"/>
   </cols>
@@ -2918,8 +3026,8 @@
   </sheetPr>
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2930,13 +3038,13 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2949,15 +3057,15 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="18" t="s">
         <v>400</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="14" t="s">
         <v>604</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="14" t="s">
         <v>404</v>
       </c>
       <c r="B5" s="10" t="s">
@@ -2965,7 +3073,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="14" t="s">
         <v>606</v>
       </c>
       <c r="B6" s="10" t="s">
@@ -2973,7 +3081,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="14" t="s">
         <v>608</v>
       </c>
       <c r="B7" s="10" t="s">
@@ -2981,7 +3089,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="14" t="s">
         <v>408</v>
       </c>
       <c r="B8" s="10" t="s">
@@ -2989,15 +3097,15 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="18" t="s">
         <v>410</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="14" t="s">
         <v>611</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="14" t="s">
         <v>414</v>
       </c>
       <c r="B11" s="10" t="s">
@@ -3005,7 +3113,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="14" t="s">
         <v>613</v>
       </c>
       <c r="B12" s="10" t="s">
@@ -3013,7 +3121,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="14" t="s">
         <v>615</v>
       </c>
       <c r="B13" s="10" t="s">
@@ -3021,7 +3129,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="14" t="s">
         <v>418</v>
       </c>
       <c r="B14" s="10" t="s">
@@ -3029,15 +3137,15 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="18" t="s">
         <v>420</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="14" t="s">
         <v>618</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="14" t="s">
         <v>424</v>
       </c>
       <c r="B17" s="10" t="s">
@@ -3045,7 +3153,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="14" t="s">
         <v>619</v>
       </c>
       <c r="B18" s="10" t="s">
@@ -3053,7 +3161,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="14" t="s">
         <v>621</v>
       </c>
       <c r="B19" s="10" t="s">
@@ -3061,7 +3169,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="14" t="s">
         <v>428</v>
       </c>
       <c r="B20" s="10" t="s">
@@ -3069,15 +3177,15 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="20" t="s">
+      <c r="A22" s="18" t="s">
         <v>474</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="14" t="s">
         <v>624</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="14" t="s">
         <v>478</v>
       </c>
       <c r="B23" s="10" t="s">
@@ -3085,7 +3193,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="16" t="s">
+      <c r="A24" s="14" t="s">
         <v>625</v>
       </c>
       <c r="B24" s="10" t="s">
@@ -3093,7 +3201,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="16" t="s">
+      <c r="A25" s="14" t="s">
         <v>627</v>
       </c>
       <c r="B25" s="10" t="s">
@@ -3101,7 +3209,7 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="16" t="s">
+      <c r="A26" s="14" t="s">
         <v>481</v>
       </c>
       <c r="B26" s="10" t="s">
@@ -3109,15 +3217,15 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="20" t="s">
+      <c r="A28" s="18" t="s">
         <v>483</v>
       </c>
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="14" t="s">
         <v>630</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="16" t="s">
+      <c r="A29" s="14" t="s">
         <v>487</v>
       </c>
       <c r="B29" s="10" t="s">
@@ -3125,7 +3233,7 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="16" t="s">
+      <c r="A30" s="14" t="s">
         <v>631</v>
       </c>
       <c r="B30" s="10" t="s">
@@ -3133,7 +3241,7 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="16" t="s">
+      <c r="A31" s="14" t="s">
         <v>633</v>
       </c>
       <c r="B31" s="10" t="s">
@@ -3141,7 +3249,7 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="16" t="s">
+      <c r="A32" s="14" t="s">
         <v>490</v>
       </c>
       <c r="B32" s="10" t="s">
@@ -3171,6 +3279,103 @@
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="48.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>639</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.48"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>640</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -3643,7 +3848,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.71"/>
   </cols>
   <sheetData>
@@ -4535,7 +4740,7 @@
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.71"/>
   </cols>
   <sheetData>
@@ -5130,7 +5335,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="71.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.71"/>
   </cols>
@@ -5146,38 +5351,38 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" s="15" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>306</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="C2" s="14"/>
-    </row>
-    <row r="3" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="14" t="s">
         <v>400</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="14" t="s">
         <v>401</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="14" t="s">
         <v>402</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="15" t="s">
         <v>403</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="14" t="s">
         <v>404</v>
       </c>
       <c r="B6" s="10" t="s">
@@ -5185,7 +5390,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="14" t="s">
         <v>406</v>
       </c>
       <c r="B7" s="10" t="s">
@@ -5193,7 +5398,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="14" t="s">
         <v>408</v>
       </c>
       <c r="B8" s="10" t="s">
@@ -5201,27 +5406,27 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="16"/>
+      <c r="A9" s="14"/>
       <c r="B9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="14" t="s">
         <v>410</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="14" t="s">
         <v>411</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="14" t="s">
         <v>412</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="14" t="s">
         <v>413</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="14" t="s">
         <v>414</v>
       </c>
       <c r="B12" s="10" t="s">
@@ -5229,7 +5434,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="165" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="14" t="s">
         <v>416</v>
       </c>
       <c r="B13" s="13" t="s">
@@ -5237,7 +5442,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="14" t="s">
         <v>418</v>
       </c>
       <c r="B14" s="10" t="s">
@@ -5245,27 +5450,27 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="16"/>
+      <c r="A15" s="14"/>
       <c r="B15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="14" t="s">
         <v>420</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="14" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="14" t="s">
         <v>422</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="14" t="s">
         <v>423</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="14" t="s">
         <v>424</v>
       </c>
       <c r="B18" s="10" t="s">
@@ -5273,7 +5478,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="132" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="14" t="s">
         <v>426</v>
       </c>
       <c r="B19" s="13" t="s">
@@ -5281,7 +5486,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="14" t="s">
         <v>428</v>
       </c>
       <c r="B20" s="10" t="s">
@@ -5312,7 +5517,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="68.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.71"/>
   </cols>
@@ -5512,18 +5717,18 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="64.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="32.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="32.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="10" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
     </row>
@@ -5547,7 +5752,7 @@
       <c r="A5" s="10" t="s">
         <v>463</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="17" t="s">
         <v>464</v>
       </c>
     </row>
@@ -5587,7 +5792,7 @@
       <c r="A11" s="10" t="s">
         <v>467</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="17" t="s">
         <v>468</v>
       </c>
     </row>
@@ -5627,7 +5832,7 @@
       <c r="A17" s="10" t="s">
         <v>471</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="17" t="s">
         <v>472</v>
       </c>
     </row>
@@ -5667,7 +5872,7 @@
       <c r="A23" s="10" t="s">
         <v>476</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="17" t="s">
         <v>477</v>
       </c>
     </row>
@@ -5707,7 +5912,7 @@
       <c r="A29" s="10" t="s">
         <v>485</v>
       </c>
-      <c r="B29" s="19" t="s">
+      <c r="B29" s="17" t="s">
         <v>486</v>
       </c>
     </row>
@@ -5747,7 +5952,7 @@
       <c r="A35" s="10" t="s">
         <v>494</v>
       </c>
-      <c r="B35" s="19" t="s">
+      <c r="B35" s="17" t="s">
         <v>464</v>
       </c>
     </row>
@@ -5787,7 +5992,7 @@
       <c r="A41" s="10" t="s">
         <v>501</v>
       </c>
-      <c r="B41" s="19" t="s">
+      <c r="B41" s="17" t="s">
         <v>468</v>
       </c>
     </row>
@@ -5827,7 +6032,7 @@
       <c r="A47" s="10" t="s">
         <v>508</v>
       </c>
-      <c r="B47" s="19" t="s">
+      <c r="B47" s="17" t="s">
         <v>472</v>
       </c>
     </row>
@@ -5867,7 +6072,7 @@
       <c r="A53" s="10" t="s">
         <v>515</v>
       </c>
-      <c r="B53" s="19" t="s">
+      <c r="B53" s="17" t="s">
         <v>477</v>
       </c>
     </row>
@@ -5907,7 +6112,7 @@
       <c r="A59" s="10" t="s">
         <v>522</v>
       </c>
-      <c r="B59" s="19" t="s">
+      <c r="B59" s="17" t="s">
         <v>486</v>
       </c>
     </row>
@@ -5947,7 +6152,7 @@
       <c r="A65" s="10" t="s">
         <v>529</v>
       </c>
-      <c r="B65" s="19" t="s">
+      <c r="B65" s="17" t="s">
         <v>464</v>
       </c>
     </row>
@@ -5987,7 +6192,7 @@
       <c r="A71" s="10" t="s">
         <v>536</v>
       </c>
-      <c r="B71" s="19" t="s">
+      <c r="B71" s="17" t="s">
         <v>537</v>
       </c>
     </row>
@@ -6027,7 +6232,7 @@
       <c r="A77" s="10" t="s">
         <v>544</v>
       </c>
-      <c r="B77" s="19" t="s">
+      <c r="B77" s="17" t="s">
         <v>545</v>
       </c>
     </row>
@@ -6067,7 +6272,7 @@
       <c r="A83" s="10" t="s">
         <v>552</v>
       </c>
-      <c r="B83" s="19" t="s">
+      <c r="B83" s="17" t="s">
         <v>553</v>
       </c>
     </row>
@@ -6107,7 +6312,7 @@
       <c r="A89" s="10" t="s">
         <v>560</v>
       </c>
-      <c r="B89" s="19" t="s">
+      <c r="B89" s="17" t="s">
         <v>561</v>
       </c>
     </row>
@@ -6147,7 +6352,7 @@
       <c r="A95" s="10" t="s">
         <v>568</v>
       </c>
-      <c r="B95" s="19" t="s">
+      <c r="B95" s="17" t="s">
         <v>537</v>
       </c>
     </row>
@@ -6187,7 +6392,7 @@
       <c r="A101" s="10" t="s">
         <v>575</v>
       </c>
-      <c r="B101" s="19" t="s">
+      <c r="B101" s="17" t="s">
         <v>576</v>
       </c>
     </row>
@@ -6227,7 +6432,7 @@
       <c r="A107" s="10" t="s">
         <v>583</v>
       </c>
-      <c r="B107" s="19" t="s">
+      <c r="B107" s="17" t="s">
         <v>584</v>
       </c>
     </row>
@@ -6267,7 +6472,7 @@
       <c r="A113" s="10" t="s">
         <v>591</v>
       </c>
-      <c r="B113" s="19" t="s">
+      <c r="B113" s="17" t="s">
         <v>477</v>
       </c>
     </row>
@@ -6307,7 +6512,7 @@
       <c r="A119" s="10" t="s">
         <v>598</v>
       </c>
-      <c r="B119" s="19" t="s">
+      <c r="B119" s="17" t="s">
         <v>486</v>
       </c>
     </row>

</xml_diff>

<commit_message>
* link case study
</commit_message>
<xml_diff>
--- a/data/text.xlsx
+++ b/data/text.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="659">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="664">
   <si>
     <t xml:space="preserve">::ID::</t>
   </si>
@@ -1268,6 +1268,12 @@
     <t xml:space="preserve">SECTION_4_LOGO_1</t>
   </si>
   <si>
+    <t xml:space="preserve">IMAGE::CASE_STUDY_LOGO_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SECTION_4_TEXT_1</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -1276,7 +1282,57 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">IMAGE::</t>
+      <t xml:space="preserve">Whenever having a chance to work with</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF5B9BD5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;span className='{{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00A65D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">custom</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF5B9BD5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">}}'&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFAA61A"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Nekodesign</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF5B9BD5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;/span&gt;</t>
     </r>
     <r>
       <rPr>
@@ -1284,12 +1340,19 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">CASE_STUDY_LOGO_5</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">SECTION_4_TEXT_1</t>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, I’m so satisfied with their abilities. Every final artwork they did always showed the highest creativity and dedication of the Team. One of the project kinds that impressed me the most is creating characters in illustrator.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">SECTION_4_TITLE_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Justin Tung - Account Manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SECTION_4_LINK_1</t>
   </si>
   <si>
     <r>
@@ -1300,95 +1363,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Whenever having a chance to work with</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF5B9BD5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> &lt;span className=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF5B9BD5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF5B9BD5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">{{</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00A65D"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">custom</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF5B9BD5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">}}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF5B9BD5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF5B9BD5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFAA61A"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Nekodesign</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF5B9BD5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;/span&gt;</t>
+      <t xml:space="preserve">LINK::</t>
     </r>
     <r>
       <rPr>
@@ -1396,43 +1371,15 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">, I’m so satisfied with their abilities. Every final artwork they did always showed the highest creativity and dedication of the Team. One of the project kinds that impressed me the most is creating characters in illustrator.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">SECTION_4_TITLE_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Justin Tung - Account Manager</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SECTION_4_LINK_1</t>
+      </rPr>
+      <t xml:space="preserve">CASE_STUDY_1</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">SECTION_4_LOGO_2</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">IMAGE::</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">CASE_STUDY_LOGO_1</t>
-    </r>
+    <t xml:space="preserve">IMAGE::CASE_STUDY_LOGO_1</t>
   </si>
   <si>
     <t xml:space="preserve">SECTION_4_TEXT_2</t>
@@ -1454,6 +1401,7 @@
         <color rgb="FF5B9BD5"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">&lt;span className='{{</t>
     </r>
@@ -1463,6 +1411,7 @@
         <color rgb="FF00A65D"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">custom</t>
     </r>
@@ -1472,6 +1421,7 @@
         <color rgb="FF5B9BD5"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">}}'&gt;</t>
     </r>
@@ -1481,6 +1431,7 @@
         <color rgb="FFFAA61A"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Nekodesign</t>
     </r>
@@ -1490,6 +1441,7 @@
         <color rgb="FF5B9BD5"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">&lt;/span&gt;</t>
     </r>
@@ -1514,28 +1466,31 @@
     <t xml:space="preserve">SECTION_4_LINK_2</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">LINK::</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">CASE_STUDY_2</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">SECTION_4_LOGO_3</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">IMAGE::</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">CASE_STUDY_LOGO_4</t>
-    </r>
+    <t xml:space="preserve">IMAGE::CASE_STUDY_LOGO_4</t>
   </si>
   <si>
     <t xml:space="preserve">SECTION_4_TEXT_3</t>
@@ -1547,6 +1502,7 @@
         <color rgb="FF5B9BD5"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">&lt;span className='{{</t>
     </r>
@@ -1556,6 +1512,7 @@
         <color rgb="FF00A65D"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">custom</t>
     </r>
@@ -1565,6 +1522,7 @@
         <color rgb="FF5B9BD5"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">}}'&gt;</t>
     </r>
@@ -1574,6 +1532,7 @@
         <color rgb="FFFAA61A"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Nekodesign</t>
     </r>
@@ -1583,6 +1542,7 @@
         <color rgb="FF5B9BD5"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">&lt;/span&gt;</t>
     </r>
@@ -1607,28 +1567,31 @@
     <t xml:space="preserve">SECTION_4_LINK_3</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">LINK::</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">CASE_STUDY_3</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">SECTION_4_LOGO_4</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">IMAGE::</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">CASE_STUDY_LOGO_3</t>
-    </r>
+    <t xml:space="preserve">IMAGE::CASE_STUDY_LOGO_3</t>
   </si>
   <si>
     <t xml:space="preserve">SECTION_4_TEXT_4</t>
@@ -1640,6 +1603,7 @@
         <color rgb="FF5B9BD5"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">&lt;span className='{{</t>
     </r>
@@ -1649,6 +1613,7 @@
         <color rgb="FF00A65D"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">custom</t>
     </r>
@@ -1658,6 +1623,7 @@
         <color rgb="FF5B9BD5"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">}}'&gt;</t>
     </r>
@@ -1667,6 +1633,7 @@
         <color rgb="FFFAA61A"/>
         <rFont val="Open Sans"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Quan and his team</t>
     </r>
@@ -1676,6 +1643,7 @@
         <color rgb="FF5B9BD5"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">&lt;/span&gt;</t>
     </r>
@@ -1700,28 +1668,31 @@
     <t xml:space="preserve">SECTION_4_LINK_4</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">LINK::</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">CASE_STUDY_4</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">SECTION_4_LOGO_5</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">IMAGE::</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">CASE_STUDY_LOGO_2</t>
-    </r>
+    <t xml:space="preserve">IMAGE::CASE_STUDY_LOGO_2</t>
   </si>
   <si>
     <t xml:space="preserve">SECTION_4_TEXT_5</t>
@@ -1743,6 +1714,7 @@
         <color rgb="FF5B9BD5"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">&lt;span className='{{</t>
     </r>
@@ -1752,6 +1724,7 @@
         <color rgb="FF00A65D"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">custom</t>
     </r>
@@ -1761,6 +1734,7 @@
         <color rgb="FF5B9BD5"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">}}'&gt;</t>
     </r>
@@ -1770,6 +1744,7 @@
         <color rgb="FFFAA61A"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Nekodesign</t>
     </r>
@@ -1779,6 +1754,7 @@
         <color rgb="FF5B9BD5"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">&lt;/span&gt;</t>
     </r>
@@ -1803,12 +1779,30 @@
     <t xml:space="preserve">SECTION_4_LINK_5</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">LINK::</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">CASE_STUDY_5</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">SECTION_4_BUTTON_1</t>
   </si>
   <si>
-    <t xml:space="preserve">Read case study</t>
-  </si>
-  <si>
     <t xml:space="preserve">SECTION_4_HEADER_1</t>
   </si>
   <si>
@@ -1828,6 +1822,7 @@
         <color rgb="FF5B9BD5"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">&lt;span className='{{</t>
     </r>
@@ -1837,6 +1832,7 @@
         <color rgb="FF00A65D"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">custom</t>
     </r>
@@ -1846,6 +1842,7 @@
         <color rgb="FF5B9BD5"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">}}'&gt;</t>
     </r>
@@ -1855,6 +1852,7 @@
         <color rgb="FFFAA61A"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">trust</t>
     </r>
@@ -1864,6 +1862,7 @@
         <color rgb="FF5B9BD5"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">&lt;/span&gt;</t>
     </r>
@@ -1877,6 +1876,9 @@
       </rPr>
       <t xml:space="preserve"> Nekodesign to deliver their great brand awareness.</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">SECTION_4_BUTTON_1_LINK</t>
   </si>
   <si>
     <t xml:space="preserve">SECTION_5_TEXT_1</t>
@@ -3189,7 +3191,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="D\-MMM\-YY"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3263,22 +3265,10 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF5B9BD5"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF5B9BD5"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -3290,27 +3280,22 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Open Sans"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF00A65D"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFAA61A"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFAA61A"/>
       <name val="Open Sans"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -3430,11 +3415,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3652,100 +3637,100 @@
         <v>325</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>621</v>
+        <v>626</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
-        <v>416</v>
+        <v>421</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>622</v>
+        <v>627</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="15" t="s">
-        <v>420</v>
+        <v>425</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>623</v>
+        <v>628</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="15" t="s">
-        <v>624</v>
+        <v>629</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>625</v>
+        <v>630</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="15" t="s">
-        <v>626</v>
+        <v>631</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>627</v>
+        <v>632</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="15" t="s">
-        <v>424</v>
+        <v>429</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>628</v>
+        <v>633</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="19" t="s">
-        <v>426</v>
+        <v>431</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>629</v>
+        <v>634</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="15" t="s">
-        <v>430</v>
+        <v>435</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>630</v>
+        <v>635</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="15" t="s">
-        <v>631</v>
+        <v>636</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>632</v>
+        <v>637</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="15" t="s">
-        <v>633</v>
+        <v>638</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>634</v>
+        <v>639</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="15" t="s">
-        <v>434</v>
+        <v>439</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>635</v>
+        <v>640</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="19" t="s">
-        <v>436</v>
+        <v>441</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>636</v>
+        <v>641</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="15" t="s">
-        <v>440</v>
+        <v>445</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>280</v>
@@ -3753,39 +3738,39 @@
     </row>
     <row r="18" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="15" t="s">
-        <v>637</v>
+        <v>642</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>638</v>
+        <v>643</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="15" t="s">
-        <v>639</v>
+        <v>644</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>640</v>
+        <v>645</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="15" t="s">
-        <v>444</v>
+        <v>449</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>641</v>
+        <v>646</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="19" t="s">
-        <v>490</v>
+        <v>495</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>642</v>
+        <v>647</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="15" t="s">
-        <v>494</v>
+        <v>499</v>
       </c>
       <c r="B23" s="10" t="s">
         <v>313</v>
@@ -3793,39 +3778,39 @@
     </row>
     <row r="24" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="15" t="s">
-        <v>643</v>
+        <v>648</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>644</v>
+        <v>649</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="15" t="s">
-        <v>645</v>
+        <v>650</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>646</v>
+        <v>651</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="15" t="s">
-        <v>498</v>
+        <v>503</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>647</v>
+        <v>652</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="19" t="s">
-        <v>500</v>
+        <v>505</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>648</v>
+        <v>653</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="15" t="s">
-        <v>504</v>
+        <v>509</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>282</v>
@@ -3833,39 +3818,39 @@
     </row>
     <row r="30" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="15" t="s">
-        <v>649</v>
+        <v>654</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>650</v>
+        <v>655</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="15" t="s">
-        <v>651</v>
+        <v>656</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>652</v>
+        <v>657</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="15" t="s">
-        <v>508</v>
+        <v>513</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>653</v>
+        <v>658</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>654</v>
+        <v>659</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>656</v>
+        <v>661</v>
       </c>
       <c r="B35" s="0" t="s">
         <v>338</v>
@@ -3917,7 +3902,7 @@
         <v>325</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>657</v>
+        <v>662</v>
       </c>
     </row>
   </sheetData>
@@ -3966,7 +3951,7 @@
         <v>325</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>658</v>
+        <v>663</v>
       </c>
     </row>
   </sheetData>
@@ -3987,8 +3972,8 @@
   </sheetPr>
   <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5587,10 +5572,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C63"/>
+  <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B44" activeCellId="0" sqref="B44"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5735,268 +5720,277 @@
         <v>353</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>354</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>338</v>
+        <v>355</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="67" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>338</v>
+        <v>363</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="53.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>338</v>
+        <v>371</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>338</v>
+        <v>379</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="66.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>338</v>
+        <v>387</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>383</v>
+        <v>388</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>384</v>
+        <v>336</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="24.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
-        <v>387</v>
-      </c>
-      <c r="B46" s="0" t="s">
-        <v>388</v>
-      </c>
-    </row>
+        <v>390</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>391</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
-        <v>393</v>
-      </c>
-      <c r="B50" s="0" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>396</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>395</v>
-      </c>
-      <c r="B51" s="10" t="s">
-        <v>396</v>
+        <v>398</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>401</v>
-      </c>
-      <c r="B54" s="0" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
-        <v>403</v>
-      </c>
-      <c r="B56" s="10" t="s">
         <v>404</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>406</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
-        <v>407</v>
-      </c>
-      <c r="B59" s="10" t="s">
-        <v>408</v>
+        <v>409</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
-        <v>411</v>
-      </c>
-      <c r="B62" s="10" t="s">
-        <v>412</v>
+        <v>413</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>414</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>415</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="B63" s="10" t="s">
-        <v>414</v>
+        <v>417</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>418</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>419</v>
       </c>
     </row>
   </sheetData>
@@ -6044,7 +6038,7 @@
         <v>325</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>415</v>
+        <v>420</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -6055,42 +6049,42 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="15" t="s">
-        <v>416</v>
+        <v>421</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>417</v>
+        <v>422</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="15" t="s">
-        <v>418</v>
+        <v>423</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>419</v>
+        <v>424</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="15" t="s">
-        <v>420</v>
+        <v>425</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>421</v>
+        <v>426</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="15" t="s">
-        <v>422</v>
+        <v>427</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>423</v>
+        <v>428</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="15" t="s">
-        <v>424</v>
+        <v>429</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>425</v>
+        <v>430</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6099,42 +6093,42 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="15" t="s">
-        <v>426</v>
+        <v>431</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>427</v>
+        <v>432</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="15" t="s">
-        <v>428</v>
+        <v>433</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>429</v>
+        <v>434</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="15" t="s">
-        <v>430</v>
+        <v>435</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>431</v>
+        <v>436</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="165" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="15" t="s">
-        <v>432</v>
+        <v>437</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>433</v>
+        <v>438</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="15" t="s">
-        <v>434</v>
+        <v>439</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>435</v>
+        <v>440</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6143,42 +6137,42 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="15" t="s">
-        <v>436</v>
+        <v>441</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>437</v>
+        <v>442</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="15" t="s">
-        <v>438</v>
+        <v>443</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>439</v>
+        <v>444</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="15" t="s">
-        <v>440</v>
+        <v>445</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>441</v>
+        <v>446</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="132" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="15" t="s">
-        <v>442</v>
+        <v>447</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>443</v>
+        <v>448</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="15" t="s">
-        <v>444</v>
+        <v>449</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>445</v>
+        <v>450</v>
       </c>
     </row>
   </sheetData>
@@ -6226,7 +6220,7 @@
         <v>325</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>446</v>
+        <v>451</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6234,42 +6228,42 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>447</v>
+        <v>452</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>448</v>
+        <v>453</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>449</v>
+        <v>454</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>450</v>
+        <v>455</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>451</v>
+        <v>456</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>452</v>
+        <v>457</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>453</v>
+        <v>458</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>454</v>
+        <v>459</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>455</v>
+        <v>460</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>456</v>
+        <v>461</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6277,23 +6271,23 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>457</v>
+        <v>462</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>458</v>
+        <v>463</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>459</v>
+        <v>464</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>460</v>
+        <v>465</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>461</v>
+        <v>466</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>336</v>
@@ -6301,7 +6295,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>462</v>
+        <v>467</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>338</v>
@@ -6309,10 +6303,10 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>463</v>
+        <v>468</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>464</v>
+        <v>469</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6320,7 +6314,7 @@
         <v>342</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>465</v>
+        <v>470</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6328,55 +6322,55 @@
         <v>350</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>466</v>
+        <v>471</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>467</v>
+        <v>472</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>468</v>
+        <v>473</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>469</v>
+        <v>474</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>470</v>
+        <v>475</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>471</v>
+        <v>476</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>472</v>
+        <v>477</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>473</v>
+        <v>478</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>474</v>
+        <v>479</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>475</v>
+        <v>480</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>476</v>
+        <v>481</v>
       </c>
     </row>
   </sheetData>
@@ -6425,807 +6419,807 @@
         <v>325</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>416</v>
+        <v>421</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>478</v>
+        <v>483</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>479</v>
+        <v>484</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>480</v>
+        <v>485</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
-        <v>420</v>
+        <v>425</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>421</v>
+        <v>426</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
-        <v>422</v>
+        <v>427</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>423</v>
+        <v>428</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
-        <v>424</v>
+        <v>429</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="s">
-        <v>426</v>
+        <v>431</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="10" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>484</v>
+        <v>489</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="s">
-        <v>430</v>
+        <v>435</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>431</v>
+        <v>436</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="10" t="s">
-        <v>432</v>
+        <v>437</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>433</v>
+        <v>438</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="10" t="s">
-        <v>434</v>
+        <v>439</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="10" t="s">
-        <v>436</v>
+        <v>441</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>486</v>
+        <v>491</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="10" t="s">
-        <v>487</v>
+        <v>492</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>488</v>
+        <v>493</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="s">
-        <v>440</v>
+        <v>445</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>441</v>
+        <v>446</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="s">
-        <v>442</v>
+        <v>447</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>443</v>
+        <v>448</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="10" t="s">
-        <v>444</v>
+        <v>449</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>489</v>
+        <v>494</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="10" t="s">
-        <v>490</v>
+        <v>495</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>491</v>
+        <v>496</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="10" t="s">
-        <v>492</v>
+        <v>497</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>493</v>
+        <v>498</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="10" t="s">
-        <v>494</v>
+        <v>499</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>495</v>
+        <v>500</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="247.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="10" t="s">
-        <v>496</v>
+        <v>501</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>497</v>
+        <v>502</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="10" t="s">
-        <v>498</v>
+        <v>503</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>499</v>
+        <v>504</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="10" t="s">
-        <v>500</v>
+        <v>505</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>501</v>
+        <v>506</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="10" t="s">
-        <v>502</v>
+        <v>507</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>503</v>
+        <v>508</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="10" t="s">
-        <v>504</v>
+        <v>509</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>505</v>
+        <v>510</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="165" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="10" t="s">
-        <v>506</v>
+        <v>511</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>507</v>
+        <v>512</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="10" t="s">
-        <v>508</v>
+        <v>513</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>509</v>
+        <v>514</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="10" t="s">
-        <v>510</v>
+        <v>515</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>511</v>
+        <v>516</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="10" t="s">
-        <v>512</v>
+        <v>517</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>480</v>
+        <v>485</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="10" t="s">
-        <v>513</v>
+        <v>518</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>421</v>
+        <v>426</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="10" t="s">
-        <v>514</v>
+        <v>519</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>423</v>
+        <v>428</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="10" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="10" t="s">
-        <v>517</v>
+        <v>522</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>518</v>
+        <v>523</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="10" t="s">
-        <v>519</v>
+        <v>524</v>
       </c>
       <c r="B41" s="18" t="s">
-        <v>484</v>
+        <v>489</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="10" t="s">
-        <v>520</v>
+        <v>525</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>431</v>
+        <v>436</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="10" t="s">
-        <v>521</v>
+        <v>526</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>433</v>
+        <v>438</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="10" t="s">
-        <v>522</v>
+        <v>527</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>523</v>
+        <v>528</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="10" t="s">
-        <v>524</v>
+        <v>529</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>525</v>
+        <v>530</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="10" t="s">
-        <v>526</v>
+        <v>531</v>
       </c>
       <c r="B47" s="18" t="s">
-        <v>488</v>
+        <v>493</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="10" t="s">
-        <v>527</v>
+        <v>532</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>441</v>
+        <v>446</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="10" t="s">
-        <v>528</v>
+        <v>533</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>443</v>
+        <v>448</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="10" t="s">
-        <v>529</v>
+        <v>534</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>530</v>
+        <v>535</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="10" t="s">
-        <v>531</v>
+        <v>536</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>532</v>
+        <v>537</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="10" t="s">
-        <v>533</v>
+        <v>538</v>
       </c>
       <c r="B53" s="18" t="s">
-        <v>493</v>
+        <v>498</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="10" t="s">
-        <v>534</v>
+        <v>539</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>495</v>
+        <v>500</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="247.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="10" t="s">
-        <v>535</v>
+        <v>540</v>
       </c>
       <c r="B55" s="13" t="s">
-        <v>497</v>
+        <v>502</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="10" t="s">
-        <v>536</v>
+        <v>541</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>537</v>
+        <v>542</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="10" t="s">
-        <v>538</v>
+        <v>543</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>539</v>
+        <v>544</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="10" t="s">
-        <v>540</v>
+        <v>545</v>
       </c>
       <c r="B59" s="18" t="s">
-        <v>503</v>
+        <v>508</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="10" t="s">
-        <v>541</v>
+        <v>546</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>505</v>
+        <v>510</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="165" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="10" t="s">
-        <v>542</v>
+        <v>547</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>507</v>
+        <v>512</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="10" t="s">
-        <v>543</v>
+        <v>548</v>
       </c>
       <c r="B62" s="10" t="s">
-        <v>544</v>
+        <v>549</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="10" t="s">
-        <v>545</v>
+        <v>550</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>546</v>
+        <v>551</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="10" t="s">
-        <v>547</v>
+        <v>552</v>
       </c>
       <c r="B65" s="18" t="s">
-        <v>480</v>
+        <v>485</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="10" t="s">
-        <v>548</v>
+        <v>553</v>
       </c>
       <c r="B66" s="10" t="s">
-        <v>421</v>
+        <v>426</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="10" t="s">
-        <v>549</v>
+        <v>554</v>
       </c>
       <c r="B67" s="10" t="s">
-        <v>423</v>
+        <v>428</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="10" t="s">
-        <v>550</v>
+        <v>555</v>
       </c>
       <c r="B68" s="10" t="s">
-        <v>551</v>
+        <v>556</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="10" t="s">
-        <v>552</v>
+        <v>557</v>
       </c>
       <c r="B70" s="10" t="s">
-        <v>553</v>
+        <v>558</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="10" t="s">
-        <v>554</v>
+        <v>559</v>
       </c>
       <c r="B71" s="18" t="s">
-        <v>555</v>
+        <v>560</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="10" t="s">
-        <v>556</v>
+        <v>561</v>
       </c>
       <c r="B72" s="10" t="s">
-        <v>431</v>
+        <v>436</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="10" t="s">
-        <v>557</v>
+        <v>562</v>
       </c>
       <c r="B73" s="10" t="s">
-        <v>433</v>
+        <v>438</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="10" t="s">
-        <v>558</v>
+        <v>563</v>
       </c>
       <c r="B74" s="10" t="s">
-        <v>559</v>
+        <v>564</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="10" t="s">
-        <v>560</v>
+        <v>565</v>
       </c>
       <c r="B76" s="10" t="s">
-        <v>561</v>
+        <v>566</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="10" t="s">
-        <v>562</v>
+        <v>567</v>
       </c>
       <c r="B77" s="18" t="s">
-        <v>563</v>
+        <v>568</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="10" t="s">
-        <v>564</v>
+        <v>569</v>
       </c>
       <c r="B78" s="10" t="s">
-        <v>441</v>
+        <v>446</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="10" t="s">
-        <v>565</v>
+        <v>570</v>
       </c>
       <c r="B79" s="10" t="s">
-        <v>443</v>
+        <v>448</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="10" t="s">
-        <v>566</v>
+        <v>571</v>
       </c>
       <c r="B80" s="10" t="s">
-        <v>567</v>
+        <v>572</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="10" t="s">
-        <v>568</v>
+        <v>573</v>
       </c>
       <c r="B82" s="10" t="s">
-        <v>569</v>
+        <v>574</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="10" t="s">
-        <v>570</v>
+        <v>575</v>
       </c>
       <c r="B83" s="18" t="s">
-        <v>571</v>
+        <v>576</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="10" t="s">
-        <v>572</v>
+        <v>577</v>
       </c>
       <c r="B84" s="10" t="s">
-        <v>495</v>
+        <v>500</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="247.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="10" t="s">
-        <v>573</v>
+        <v>578</v>
       </c>
       <c r="B85" s="13" t="s">
-        <v>497</v>
+        <v>502</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="10" t="s">
-        <v>574</v>
+        <v>579</v>
       </c>
       <c r="B86" s="10" t="s">
-        <v>575</v>
+        <v>580</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="10" t="s">
-        <v>576</v>
+        <v>581</v>
       </c>
       <c r="B88" s="10" t="s">
-        <v>577</v>
+        <v>582</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="10" t="s">
-        <v>578</v>
+        <v>583</v>
       </c>
       <c r="B89" s="18" t="s">
-        <v>579</v>
+        <v>584</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="10" t="s">
-        <v>580</v>
+        <v>585</v>
       </c>
       <c r="B90" s="10" t="s">
-        <v>505</v>
+        <v>510</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="165" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="10" t="s">
-        <v>581</v>
+        <v>586</v>
       </c>
       <c r="B91" s="13" t="s">
-        <v>507</v>
+        <v>512</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="10" t="s">
-        <v>582</v>
+        <v>587</v>
       </c>
       <c r="B92" s="10" t="s">
-        <v>583</v>
+        <v>588</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="10" t="s">
-        <v>584</v>
+        <v>589</v>
       </c>
       <c r="B94" s="10" t="s">
-        <v>585</v>
+        <v>590</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="10" t="s">
-        <v>586</v>
+        <v>591</v>
       </c>
       <c r="B95" s="18" t="s">
-        <v>555</v>
+        <v>560</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="10" t="s">
-        <v>587</v>
+        <v>592</v>
       </c>
       <c r="B96" s="10" t="s">
-        <v>421</v>
+        <v>426</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="10" t="s">
-        <v>588</v>
+        <v>593</v>
       </c>
       <c r="B97" s="10" t="s">
-        <v>423</v>
+        <v>428</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="10" t="s">
-        <v>589</v>
+        <v>594</v>
       </c>
       <c r="B98" s="10" t="s">
-        <v>590</v>
+        <v>595</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="10" t="s">
-        <v>591</v>
+        <v>596</v>
       </c>
       <c r="B100" s="10" t="s">
-        <v>592</v>
+        <v>597</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="10" t="s">
-        <v>593</v>
+        <v>598</v>
       </c>
       <c r="B101" s="18" t="s">
-        <v>594</v>
+        <v>599</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="10" t="s">
-        <v>595</v>
+        <v>600</v>
       </c>
       <c r="B102" s="10" t="s">
-        <v>431</v>
+        <v>436</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="10" t="s">
-        <v>596</v>
+        <v>601</v>
       </c>
       <c r="B103" s="10" t="s">
-        <v>433</v>
+        <v>438</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="10" t="s">
-        <v>597</v>
+        <v>602</v>
       </c>
       <c r="B104" s="10" t="s">
-        <v>598</v>
+        <v>603</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="10" t="s">
-        <v>599</v>
+        <v>604</v>
       </c>
       <c r="B106" s="10" t="s">
-        <v>600</v>
+        <v>605</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="10" t="s">
-        <v>601</v>
+        <v>606</v>
       </c>
       <c r="B107" s="18" t="s">
-        <v>602</v>
+        <v>607</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="10" t="s">
-        <v>603</v>
+        <v>608</v>
       </c>
       <c r="B108" s="10" t="s">
-        <v>441</v>
+        <v>446</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="10" t="s">
-        <v>604</v>
+        <v>609</v>
       </c>
       <c r="B109" s="10" t="s">
-        <v>443</v>
+        <v>448</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="10" t="s">
-        <v>605</v>
+        <v>610</v>
       </c>
       <c r="B110" s="10" t="s">
-        <v>606</v>
+        <v>611</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="10" t="s">
-        <v>607</v>
+        <v>612</v>
       </c>
       <c r="B112" s="10" t="s">
-        <v>608</v>
+        <v>613</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="10" t="s">
-        <v>609</v>
+        <v>614</v>
       </c>
       <c r="B113" s="18" t="s">
-        <v>493</v>
+        <v>498</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="10" t="s">
-        <v>610</v>
+        <v>615</v>
       </c>
       <c r="B114" s="10" t="s">
-        <v>495</v>
+        <v>500</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="247.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="10" t="s">
-        <v>611</v>
+        <v>616</v>
       </c>
       <c r="B115" s="13" t="s">
-        <v>497</v>
+        <v>502</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="10" t="s">
-        <v>612</v>
+        <v>617</v>
       </c>
       <c r="B116" s="10" t="s">
-        <v>613</v>
+        <v>618</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="10" t="s">
-        <v>614</v>
+        <v>619</v>
       </c>
       <c r="B118" s="10" t="s">
-        <v>615</v>
+        <v>620</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="10" t="s">
-        <v>616</v>
+        <v>621</v>
       </c>
       <c r="B119" s="18" t="s">
-        <v>503</v>
+        <v>508</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="10" t="s">
-        <v>617</v>
+        <v>622</v>
       </c>
       <c r="B120" s="10" t="s">
-        <v>505</v>
+        <v>510</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="165" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="10" t="s">
-        <v>618</v>
+        <v>623</v>
       </c>
       <c r="B121" s="13" t="s">
-        <v>507</v>
+        <v>512</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="10" t="s">
-        <v>619</v>
+        <v>624</v>
       </c>
       <c r="B122" s="10" t="s">
-        <v>620</v>
+        <v>625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
+ streamline section 2
</commit_message>
<xml_diff>
--- a/data/text.xlsx
+++ b/data/text.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\ReactJS\_neko_website\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE03B2E9-B22F-4A62-BC40-B9B7F799105A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6674158-63A0-4BD4-A786-D1CB82753A83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="930" windowWidth="21600" windowHeight="11385" tabRatio="851" firstSheet="7" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="851" firstSheet="1" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COMMON" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="929" uniqueCount="738">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="748">
   <si>
     <t>::ID::</t>
   </si>
@@ -3270,6 +3270,36 @@
   </si>
   <si>
     <t>Don't hesitate to contact us. We'll get in touch with you within 24 hours after receiving your information.</t>
+  </si>
+  <si>
+    <t>SECTION_2_IMG_3</t>
+  </si>
+  <si>
+    <t>STREAMLINE_1</t>
+  </si>
+  <si>
+    <t>STREAMLINE_2</t>
+  </si>
+  <si>
+    <t>STREAMLINE_3</t>
+  </si>
+  <si>
+    <t>/images/streamline/time.png</t>
+  </si>
+  <si>
+    <t>/images/streamline/task.png</t>
+  </si>
+  <si>
+    <t>/images/streamline/money.png</t>
+  </si>
+  <si>
+    <t>IMAGE::STREAMLINE_2</t>
+  </si>
+  <si>
+    <t>IMAGE::STREAMLINE_3</t>
+  </si>
+  <si>
+    <t>IMAGE::STREAMLINE_1</t>
   </si>
 </sst>
 </file>
@@ -4255,10 +4285,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4354,102 +4384,126 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>720</v>
+        <v>462</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>724</v>
+        <v>747</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>720</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>721</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B14" s="20" t="s">
         <v>725</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>722</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>727</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>470</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>722</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>723</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B17" s="20" t="s">
         <v>726</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>344</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>728</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>729</v>
+        <v>738</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>730</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>461</v>
+        <v>746</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>344</v>
+      </c>
       <c r="B20" s="20" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>352</v>
+        <v>729</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>732</v>
+        <v>459</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>730</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="20" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>352</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>360</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B25" s="20" t="s">
         <v>734</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="26" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>368</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="B26" s="20" t="s">
         <v>733</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="28" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>394</v>
       </c>
-      <c r="B25" s="20" t="s">
+      <c r="B28" s="20" t="s">
         <v>735</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="29" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>736</v>
       </c>
-      <c r="B26" s="20" t="s">
+      <c r="B29" s="20" t="s">
         <v>737</v>
       </c>
     </row>
@@ -5108,10 +5162,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C93"/>
+  <dimension ref="A1:C97"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView topLeftCell="A82" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A96" sqref="A96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5781,7 +5835,32 @@
         <v>144</v>
       </c>
     </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>739</v>
+      </c>
+      <c r="B95" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>740</v>
+      </c>
+      <c r="B96" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>741</v>
+      </c>
+      <c r="B97" t="s">
+        <v>744</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>

<commit_message>
* Feedback HOME spcialize smaller * Feedback HOME 85 project anim
</commit_message>
<xml_diff>
--- a/data/text.xlsx
+++ b/data/text.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="COMMON" sheetId="1" state="visible" r:id="rId2"/>
@@ -962,97 +962,100 @@
     <t xml:space="preserve">Brand Identity</t>
   </si>
   <si>
+    <t xml:space="preserve">Motion/Animation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User Interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2D Graphics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digital Project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WORKS_BRAND_BG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rgb(186, 132, 132)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WORKS_MOTION_BG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rgb(213, 207, 233)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WORKS_INTERFACE_BG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rgb(165, 181, 206)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WORKS_GRAPHICS_BG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rgb(162, 138, 104)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WORKS_DIGITAL_BG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rgb(120, 182, 169)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SECONDARY_TITLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Let's make it live.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SECONDARY_SUBTITLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">start a cooperation with us</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRIMARY_COPYRIGHT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">© 2020 Nekodesign. All rights reserved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRIMARY_CONTACT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Looking for the inspiration for your next project:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRIMARY_CONTACT_EMAIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e: quan.nguyen@nekodesign.asia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRIMARY_CONTACT_PHONE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m: +84 38 849 1985</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRIMARY_WORKS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WOKS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRIMARY_WORKS_BRAND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Branding Identity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRIMARY_WORKS_MOTION</t>
+  </si>
+  <si>
     <t xml:space="preserve">Motion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User Interface</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2D Graphics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Digital Project</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WORKS_BRAND_BG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rgb(186, 132, 132)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WORKS_MOTION_BG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rgb(213, 207, 233)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WORKS_INTERFACE_BG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rgb(165, 181, 206)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WORKS_GRAPHICS_BG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rgb(162, 138, 104)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WORKS_DIGITAL_BG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rgb(120, 182, 169)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SECONDARY_TITLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Let's make it live.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SECONDARY_SUBTITLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">start a cooperation with us</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRIMARY_COPYRIGHT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">© 2020 Nekodesign. All rights reserved</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRIMARY_CONTACT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Looking for the inspiration for your next project:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRIMARY_CONTACT_EMAIL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">e: quan.nguyen@nekodesign.asia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRIMARY_CONTACT_PHONE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">m: +84 38 849 1985</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRIMARY_WORKS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WOKS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRIMARY_WORKS_BRAND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Branding Identity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRIMARY_WORKS_MOTION</t>
   </si>
   <si>
     <t xml:space="preserve">PRIMARY_WORKS_WEB</t>
@@ -2920,9 +2923,6 @@
   </si>
   <si>
     <t xml:space="preserve">IMAGE::CAPABILITIES_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Motion/Animation</t>
   </si>
   <si>
     <t xml:space="preserve">DESCRIPTION_2</t>
@@ -3747,66 +3747,66 @@
     </row>
     <row r="2" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="15" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="15" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="15" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="15" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="19" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="15" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>643</v>
+        <v>287</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3827,7 +3827,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="15" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>648</v>
@@ -3835,7 +3835,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="19" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="B16" s="15" t="s">
         <v>649</v>
@@ -3843,7 +3843,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="15" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>288</v>
@@ -3867,7 +3867,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="15" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>654</v>
@@ -3875,7 +3875,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="19" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B22" s="15" t="s">
         <v>655</v>
@@ -3883,10 +3883,10 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="15" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3907,7 +3907,7 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="15" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>660</v>
@@ -3915,7 +3915,7 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="19" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="B28" s="15" t="s">
         <v>661</v>
@@ -3923,7 +3923,7 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="15" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>290</v>
@@ -3947,7 +3947,7 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="15" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B32" s="10" t="s">
         <v>666</v>
@@ -3966,7 +3966,7 @@
         <v>669</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
   </sheetData>
@@ -4012,7 +4012,7 @@
     </row>
     <row r="2" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>670</v>
@@ -4020,7 +4020,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>671</v>
@@ -4104,7 +4104,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>680</v>
@@ -4112,7 +4112,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B3" s="20" t="s">
         <v>681</v>
@@ -4120,7 +4120,7 @@
     </row>
     <row r="4" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B4" s="20" t="s">
         <v>682</v>
@@ -4136,7 +4136,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B6" s="20" t="s">
         <v>685</v>
@@ -4147,7 +4147,7 @@
         <v>686</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4176,7 +4176,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="B12" s="20" t="s">
         <v>693</v>
@@ -4200,7 +4200,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="B15" s="20" t="s">
         <v>698</v>
@@ -4232,7 +4232,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B20" s="20" t="s">
         <v>705</v>
@@ -4243,7 +4243,7 @@
         <v>706</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4251,7 +4251,7 @@
         <v>707</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4261,7 +4261,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B24" s="20" t="s">
         <v>709</v>
@@ -4269,7 +4269,7 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B25" s="20" t="s">
         <v>710</v>
@@ -4277,7 +4277,7 @@
     </row>
     <row r="26" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B26" s="20" t="s">
         <v>711</v>
@@ -4285,7 +4285,7 @@
     </row>
     <row r="28" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B28" s="20" t="s">
         <v>712</v>
@@ -4358,7 +4358,7 @@
     </row>
     <row r="5" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B5" s="20" t="s">
         <v>718</v>
@@ -4390,15 +4390,15 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B11" s="20" t="s">
         <v>725</v>
@@ -5685,8 +5685,8 @@
   </sheetPr>
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6060,28 +6060,28 @@
         <v>317</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>287</v>
+        <v>318</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>290</v>
@@ -6089,42 +6089,42 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -6145,7 +6145,7 @@
   </sheetPr>
   <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
     </sheetView>
   </sheetViews>
@@ -6170,71 +6170,71 @@
     </row>
     <row r="2" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B12" s="5" t="n">
         <v>85</v>
@@ -6242,26 +6242,26 @@
     </row>
     <row r="13" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B16" s="5" t="n">
         <v>5</v>
@@ -6269,298 +6269,298 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="99" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="66" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="82.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="99" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B63" s="10" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
   </sheetData>
@@ -6605,10 +6605,10 @@
     </row>
     <row r="2" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -6619,42 +6619,42 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="15" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="15" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="15" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="15" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="15" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6663,42 +6663,42 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="15" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="15" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="15" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="165" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="15" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="15" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6707,42 +6707,42 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="15" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="15" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="15" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="132" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="15" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="15" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
   </sheetData>
@@ -6763,7 +6763,7 @@
   </sheetPr>
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -6787,10 +6787,10 @@
     </row>
     <row r="2" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6798,42 +6798,42 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6841,106 +6841,106 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
   </sheetData>
@@ -6986,810 +6986,810 @@
     </row>
     <row r="2" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="10" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="10" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="10" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="10" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="10" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="10" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="10" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="10" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="10" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="247.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="10" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="10" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="10" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="10" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="10" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="165" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="10" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="10" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="10" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="10" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="10" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="10" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="10" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="10" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="10" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="B41" s="18" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="10" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="10" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="10" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="10" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="10" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="B47" s="18" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="10" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="10" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="10" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="10" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="10" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="B53" s="18" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="10" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="247.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="10" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="B55" s="13" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="10" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="10" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="10" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="B59" s="18" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="10" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="165" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="10" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="10" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="B62" s="10" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="10" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="10" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="B65" s="18" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="10" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="B66" s="10" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="10" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="B67" s="10" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="10" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="B68" s="10" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="10" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="B70" s="10" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="10" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="B71" s="18" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="10" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="B72" s="10" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="10" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="B73" s="10" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="10" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="B74" s="10" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="10" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="B76" s="10" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="10" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="B77" s="18" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="10" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="B78" s="10" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="10" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="B79" s="10" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="10" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="B80" s="10" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="10" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="B82" s="10" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="10" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="B83" s="18" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="10" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="B84" s="10" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="247.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="10" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="B85" s="13" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="10" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="B86" s="10" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="10" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B88" s="10" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="10" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="B89" s="18" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="10" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="B90" s="10" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="165" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="10" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="B91" s="13" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="10" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="B92" s="10" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="10" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="B94" s="10" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="10" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="B95" s="18" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="10" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="B96" s="10" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="10" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="B97" s="10" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="10" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="B98" s="10" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="10" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="B100" s="10" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="10" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="B101" s="18" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="10" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="B102" s="10" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="10" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="B103" s="10" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="10" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="B104" s="10" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="10" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="B106" s="10" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="10" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="B107" s="18" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="10" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="B108" s="10" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="10" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="B109" s="10" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="10" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="B110" s="10" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="10" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="B112" s="10" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="10" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="B113" s="18" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="10" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="B114" s="10" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="247.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="10" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="B115" s="13" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="10" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="B116" s="10" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="10" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="B118" s="10" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="10" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="B119" s="18" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="10" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="B120" s="10" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="165" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="10" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="B121" s="13" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="10" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="B122" s="10" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* feedback HOME case study * feedback FOOTER streamline
</commit_message>
<xml_diff>
--- a/data/text.xlsx
+++ b/data/text.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="COMMON" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="748">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="760">
   <si>
     <t xml:space="preserve">::ID::</t>
   </si>
@@ -612,6 +612,12 @@
   </si>
   <si>
     <t xml:space="preserve">/images/home/85++.svg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HOME_4_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/images/home/stars.svg</t>
   </si>
   <si>
     <t xml:space="preserve">HOME_4_2</t>
@@ -1377,7 +1383,13 @@
     <t xml:space="preserve">SECTION_4_TITLE_1</t>
   </si>
   <si>
-    <t xml:space="preserve">Justin Tung - Account Manager</t>
+    <t xml:space="preserve">Justin Tung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SECTION_4_SUBTITLE_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Account Manager</t>
   </si>
   <si>
     <t xml:space="preserve">SECTION_4_LINK_1</t>
@@ -1470,7 +1482,13 @@
     <t xml:space="preserve">SECTION_4_TITLE_2</t>
   </si>
   <si>
-    <t xml:space="preserve">Nguyen Huu Viet Hai - Senior PR Account</t>
+    <t xml:space="preserve">Nguyen Huu Viet Hai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SECTION_4_SUBTITLE_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Senior PR Account</t>
   </si>
   <si>
     <t xml:space="preserve">SECTION_4_LINK_2</t>
@@ -1553,7 +1571,13 @@
     <t xml:space="preserve">SECTION_4_TITLE_3</t>
   </si>
   <si>
-    <t xml:space="preserve">Andrey Pafilov - Co-owner &amp; VFX lead artist</t>
+    <t xml:space="preserve">Andrey Pafilov</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SECTION_4_SUBTITLE_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Co-owner &amp; VFX lead artist</t>
   </si>
   <si>
     <t xml:space="preserve">SECTION_4_LINK_3</t>
@@ -1636,7 +1660,13 @@
     <t xml:space="preserve">SECTION_4_TITLE_4</t>
   </si>
   <si>
-    <t xml:space="preserve">Cecilia Ang - Executive Producer</t>
+    <t xml:space="preserve">Cecilia Ang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SECTION_4_SUBTITLE_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Executive Producer</t>
   </si>
   <si>
     <t xml:space="preserve">SECTION_4_LINK_4</t>
@@ -1729,7 +1759,13 @@
     <t xml:space="preserve">SECTION_4_TITLE_5</t>
   </si>
   <si>
-    <t xml:space="preserve">Nguyen Thi Thuy Linh - Video Editor</t>
+    <t xml:space="preserve">Nguyen Thi Thuy Linh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SECTION_4_SUBTITLE_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Video Editor</t>
   </si>
   <si>
     <t xml:space="preserve">SECTION_4_LINK_5</t>
@@ -3306,7 +3342,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="D\-MMM\-YY"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3395,6 +3431,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Open Sans"/>
       <family val="2"/>
       <charset val="1"/>
@@ -3471,7 +3513,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3524,7 +3566,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3735,238 +3781,238 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>635</v>
+        <v>647</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="19" t="s">
-        <v>430</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>636</v>
+      <c r="A4" s="20" t="s">
+        <v>442</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>648</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="15" t="s">
-        <v>434</v>
+      <c r="A5" s="16" t="s">
+        <v>446</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>637</v>
+        <v>649</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="15" t="s">
-        <v>638</v>
+      <c r="A6" s="16" t="s">
+        <v>650</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>639</v>
+        <v>651</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="15" t="s">
-        <v>640</v>
+      <c r="A7" s="16" t="s">
+        <v>652</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>641</v>
+        <v>653</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="15" t="s">
-        <v>438</v>
+      <c r="A8" s="16" t="s">
+        <v>450</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>642</v>
+        <v>654</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="19" t="s">
-        <v>440</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>643</v>
+      <c r="A10" s="20" t="s">
+        <v>452</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>655</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="15" t="s">
-        <v>444</v>
+      <c r="A11" s="16" t="s">
+        <v>456</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="15" t="s">
-        <v>644</v>
+      <c r="A12" s="16" t="s">
+        <v>656</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>645</v>
+        <v>657</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="15" t="s">
-        <v>646</v>
+      <c r="A13" s="16" t="s">
+        <v>658</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>647</v>
+        <v>659</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="15" t="s">
-        <v>448</v>
+      <c r="A14" s="16" t="s">
+        <v>460</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>648</v>
+        <v>660</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="19" t="s">
-        <v>450</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>649</v>
+      <c r="A16" s="20" t="s">
+        <v>462</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>661</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="15" t="s">
-        <v>454</v>
+      <c r="A17" s="16" t="s">
+        <v>466</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="15" t="s">
-        <v>650</v>
+      <c r="A18" s="16" t="s">
+        <v>662</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>651</v>
+        <v>663</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="15" t="s">
-        <v>652</v>
+      <c r="A19" s="16" t="s">
+        <v>664</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>653</v>
+        <v>665</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="15" t="s">
-        <v>458</v>
+      <c r="A20" s="16" t="s">
+        <v>470</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>654</v>
+        <v>666</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="19" t="s">
-        <v>504</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>655</v>
+      <c r="A22" s="20" t="s">
+        <v>516</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>667</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="15" t="s">
-        <v>508</v>
+      <c r="A23" s="16" t="s">
+        <v>520</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="15" t="s">
-        <v>656</v>
+      <c r="A24" s="16" t="s">
+        <v>668</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>657</v>
+        <v>669</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="15" t="s">
-        <v>658</v>
+      <c r="A25" s="16" t="s">
+        <v>670</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>659</v>
+        <v>671</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="15" t="s">
-        <v>512</v>
+      <c r="A26" s="16" t="s">
+        <v>524</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>660</v>
+        <v>672</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="19" t="s">
-        <v>514</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>661</v>
+      <c r="A28" s="20" t="s">
+        <v>526</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>673</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="15" t="s">
-        <v>518</v>
+      <c r="A29" s="16" t="s">
+        <v>530</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="15" t="s">
-        <v>662</v>
+      <c r="A30" s="16" t="s">
+        <v>674</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>663</v>
+        <v>675</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="15" t="s">
-        <v>664</v>
+      <c r="A31" s="16" t="s">
+        <v>676</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>665</v>
+        <v>677</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="15" t="s">
-        <v>522</v>
+      <c r="A32" s="16" t="s">
+        <v>534</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>666</v>
+        <v>678</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>667</v>
+        <v>679</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>668</v>
+        <v>680</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>669</v>
+        <v>681</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
     </row>
   </sheetData>
@@ -4000,62 +4046,62 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>670</v>
+        <v>682</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>671</v>
+        <v>683</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>672</v>
+        <v>684</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>673</v>
+        <v>685</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>674</v>
+        <v>686</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>675</v>
+        <v>687</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>676</v>
+        <v>688</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>677</v>
+        <v>689</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>678</v>
+        <v>690</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>679</v>
+        <v>691</v>
       </c>
     </row>
   </sheetData>
@@ -4086,217 +4132,217 @@
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="50.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="21" width="50.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>680</v>
+        <v>692</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>336</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>681</v>
+        <v>338</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>338</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>682</v>
+        <v>340</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>694</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>683</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>684</v>
+        <v>695</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>696</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>685</v>
+        <v>342</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>697</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>686</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>347</v>
+        <v>698</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>687</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>688</v>
+        <v>699</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>700</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>689</v>
-      </c>
-      <c r="B10" s="20" t="s">
-        <v>690</v>
+        <v>701</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>702</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>691</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>692</v>
+        <v>703</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>704</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>469</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>693</v>
+        <v>481</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>705</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>694</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>695</v>
+        <v>706</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>707</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>696</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>697</v>
+        <v>708</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>709</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>477</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>698</v>
+        <v>489</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>710</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>699</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>700</v>
+        <v>711</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>712</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>701</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>702</v>
+        <v>713</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>714</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>703</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>704</v>
+        <v>715</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>716</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>351</v>
-      </c>
-      <c r="B20" s="20" t="s">
-        <v>705</v>
+        <v>353</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>717</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>706</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>466</v>
+        <v>718</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>707</v>
-      </c>
-      <c r="B22" s="20" t="s">
-        <v>468</v>
+        <v>719</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>480</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="20" t="s">
-        <v>708</v>
+      <c r="B23" s="21" t="s">
+        <v>720</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>359</v>
-      </c>
-      <c r="B24" s="20" t="s">
-        <v>709</v>
+        <v>361</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>721</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>367</v>
-      </c>
-      <c r="B25" s="20" t="s">
-        <v>710</v>
+        <v>371</v>
+      </c>
+      <c r="B25" s="21" t="s">
+        <v>722</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>375</v>
-      </c>
-      <c r="B26" s="20" t="s">
-        <v>711</v>
+        <v>381</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>723</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>401</v>
-      </c>
-      <c r="B28" s="20" t="s">
-        <v>712</v>
+        <v>413</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>724</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>713</v>
-      </c>
-      <c r="B29" s="20" t="s">
-        <v>714</v>
+        <v>725</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>726</v>
       </c>
     </row>
   </sheetData>
@@ -4324,172 +4370,172 @@
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="39.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="21" width="39.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>715</v>
+        <v>727</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>716</v>
+        <v>728</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>687</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>717</v>
+        <v>699</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>729</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>348</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>718</v>
+        <v>350</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>730</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>719</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>720</v>
+        <v>731</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>732</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>721</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>722</v>
+        <v>733</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>734</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>723</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>724</v>
+        <v>735</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>736</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="B10" s="20" t="s">
-        <v>637</v>
+        <v>353</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>649</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>725</v>
+        <v>356</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>737</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>726</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>727</v>
+        <v>738</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>739</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>728</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>729</v>
+        <v>740</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>741</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>730</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>731</v>
+        <v>742</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>743</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>732</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>733</v>
+        <v>744</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>745</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>734</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>735</v>
+        <v>746</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>747</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>736</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>737</v>
+        <v>748</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>749</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>738</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>739</v>
+        <v>750</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>751</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>740</v>
-      </c>
-      <c r="B20" s="20" t="s">
-        <v>741</v>
+        <v>752</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>753</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>742</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>743</v>
+        <v>754</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>755</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>744</v>
-      </c>
-      <c r="B22" s="20" t="s">
-        <v>745</v>
+        <v>756</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>757</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>746</v>
-      </c>
-      <c r="B23" s="20" t="s">
-        <v>747</v>
+        <v>758</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>759</v>
       </c>
     </row>
   </sheetData>
@@ -4970,10 +5016,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C97"/>
+  <dimension ref="A1:C98"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B98" activeCellId="0" sqref="B98"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5219,7 +5265,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>171</v>
       </c>
@@ -5227,8 +5273,8 @@
         <v>172</v>
       </c>
     </row>
-    <row r="34" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="3" t="s">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
         <v>173</v>
       </c>
       <c r="B34" s="3" t="s">
@@ -5283,35 +5329,35 @@
         <v>186</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="B42" s="0" t="s">
+    <row r="41" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="3" t="s">
         <v>187</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="B44" s="0" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="B46" s="0" t="s">
+      <c r="B45" s="0" t="s">
         <v>191</v>
       </c>
     </row>
@@ -5347,171 +5393,171 @@
         <v>199</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B52" s="0" t="s">
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
         <v>200</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B71" s="0" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="B73" s="0" t="s">
+      <c r="B72" s="0" t="s">
         <v>221</v>
       </c>
     </row>
@@ -5547,35 +5593,35 @@
         <v>229</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="3" t="s">
+    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="B79" s="0" t="s">
+      <c r="B78" s="0" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="3" t="s">
+    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="B81" s="0" t="s">
+      <c r="B80" s="0" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="s">
+      <c r="A82" s="3" t="s">
         <v>234</v>
       </c>
       <c r="B82" s="0" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="s">
+    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
         <v>236</v>
       </c>
-      <c r="B84" s="0" t="s">
+      <c r="B83" s="0" t="s">
         <v>237</v>
       </c>
     </row>
@@ -5603,11 +5649,11 @@
         <v>243</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="0" t="s">
+    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
         <v>244</v>
       </c>
-      <c r="B89" s="0" t="s">
+      <c r="B88" s="0" t="s">
         <v>245</v>
       </c>
     </row>
@@ -5640,15 +5686,15 @@
         <v>252</v>
       </c>
       <c r="B93" s="0" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="B94" s="0" t="s">
         <v>144</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="0" t="s">
-        <v>253</v>
-      </c>
-      <c r="B95" s="0" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5665,6 +5711,14 @@
       </c>
       <c r="B97" s="0" t="s">
         <v>258</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="B98" s="0" t="s">
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -5685,7 +5739,7 @@
   </sheetPr>
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -5710,13 +5764,13 @@
     </row>
     <row r="2" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="3" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5736,7 +5790,7 @@
         <v>19</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5744,10 +5798,10 @@
         <v>21</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5758,7 +5812,7 @@
         <v>23</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5769,7 +5823,7 @@
         <v>25</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5789,7 +5843,7 @@
         <v>29</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5799,68 +5853,68 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5868,7 +5922,7 @@
         <v>39</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5876,7 +5930,7 @@
         <v>41</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5884,7 +5938,7 @@
         <v>43</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5892,7 +5946,7 @@
         <v>45</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5900,7 +5954,7 @@
         <v>47</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5908,47 +5962,47 @@
         <v>49</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
     </row>
   </sheetData>
@@ -5993,138 +6047,138 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
   </sheetData>
@@ -6143,10 +6197,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C64"/>
+  <dimension ref="A1:C69"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B45" activeCellId="0" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6170,71 +6224,71 @@
     </row>
     <row r="2" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="B12" s="5" t="n">
         <v>85</v>
@@ -6242,26 +6296,26 @@
     </row>
     <row r="13" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="B16" s="5" t="n">
         <v>5</v>
@@ -6269,298 +6323,338 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>363</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
         <v>365</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B21" s="13" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="99" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>367</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>369</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="99" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>369</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>371</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>372</v>
+        <v>374</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>375</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="66" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>375</v>
-      </c>
-      <c r="B29" s="14" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="66" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>379</v>
-      </c>
-      <c r="B31" s="0" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>381</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>383</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>381</v>
-      </c>
-      <c r="B33" s="0" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="82.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>385</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>383</v>
-      </c>
-      <c r="B34" s="14" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>385</v>
-      </c>
-      <c r="B35" s="0" t="s">
-        <v>386</v>
+        <v>387</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="82.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>391</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="99" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
-        <v>395</v>
-      </c>
-      <c r="B41" s="0" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="99" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>397</v>
-      </c>
-      <c r="B43" s="0" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>401</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>403</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="B45" s="0" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
-        <v>401</v>
-      </c>
-      <c r="B47" s="0" t="s">
-        <v>402</v>
+        <v>405</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>407</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>403</v>
+        <v>409</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>405</v>
-      </c>
-      <c r="B49" s="0" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
-        <v>407</v>
-      </c>
-      <c r="B51" s="0" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>410</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>412</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>409</v>
-      </c>
-      <c r="B52" s="10" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>413</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>411</v>
-      </c>
-      <c r="B53" s="10" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>415</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>413</v>
-      </c>
-      <c r="B54" s="10" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
-        <v>415</v>
-      </c>
-      <c r="B55" s="0" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>417</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>419</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>420</v>
+        <v>424</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>425</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>421</v>
-      </c>
-      <c r="B60" s="10" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
-        <v>423</v>
-      </c>
-      <c r="B61" s="10" t="s">
-        <v>424</v>
+        <v>427</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>429</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>430</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>425</v>
+        <v>431</v>
       </c>
       <c r="B63" s="10" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
-        <v>427</v>
-      </c>
-      <c r="B64" s="10" t="s">
-        <v>428</v>
+        <v>432</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>433</v>
+      </c>
+      <c r="B65" s="10" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>435</v>
+      </c>
+      <c r="B66" s="10" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>437</v>
+      </c>
+      <c r="B68" s="10" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>439</v>
+      </c>
+      <c r="B69" s="10" t="s">
+        <v>440</v>
       </c>
     </row>
   </sheetData>
@@ -6605,10 +6699,10 @@
     </row>
     <row r="2" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>429</v>
+        <v>441</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -6618,131 +6712,131 @@
       <c r="C3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="15" t="s">
-        <v>430</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>431</v>
+      <c r="A4" s="16" t="s">
+        <v>442</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>443</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="15" t="s">
-        <v>432</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>433</v>
+      <c r="A5" s="16" t="s">
+        <v>444</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="15" t="s">
-        <v>434</v>
+      <c r="A6" s="16" t="s">
+        <v>446</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>435</v>
+        <v>447</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="15" t="s">
-        <v>436</v>
+      <c r="A7" s="16" t="s">
+        <v>448</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>437</v>
+        <v>449</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="15" t="s">
-        <v>438</v>
+      <c r="A8" s="16" t="s">
+        <v>450</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>439</v>
+        <v>451</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="15"/>
+      <c r="A9" s="16"/>
       <c r="B9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="15" t="s">
-        <v>440</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>441</v>
+      <c r="A10" s="16" t="s">
+        <v>452</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="15" t="s">
-        <v>442</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>443</v>
+      <c r="A11" s="16" t="s">
+        <v>454</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>455</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="15" t="s">
-        <v>444</v>
+      <c r="A12" s="16" t="s">
+        <v>456</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>445</v>
+        <v>457</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="165" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="15" t="s">
-        <v>446</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>447</v>
+      <c r="A13" s="16" t="s">
+        <v>458</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="15" t="s">
-        <v>448</v>
+      <c r="A14" s="16" t="s">
+        <v>460</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>449</v>
+        <v>461</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="15"/>
+      <c r="A15" s="16"/>
       <c r="B15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="15" t="s">
-        <v>450</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>451</v>
+      <c r="A16" s="16" t="s">
+        <v>462</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="15" t="s">
-        <v>452</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>453</v>
+      <c r="A17" s="16" t="s">
+        <v>464</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="15" t="s">
-        <v>454</v>
+      <c r="A18" s="16" t="s">
+        <v>466</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>455</v>
+        <v>467</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="132" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="15" t="s">
-        <v>456</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>457</v>
+      <c r="A19" s="16" t="s">
+        <v>468</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>469</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="15" t="s">
-        <v>458</v>
+      <c r="A20" s="16" t="s">
+        <v>470</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
     </row>
   </sheetData>
@@ -6787,10 +6881,10 @@
     </row>
     <row r="2" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>460</v>
+        <v>472</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6798,42 +6892,42 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>461</v>
+        <v>473</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>462</v>
+        <v>474</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>463</v>
+        <v>475</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>464</v>
+        <v>476</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>465</v>
+        <v>477</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>466</v>
+        <v>478</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>467</v>
+        <v>479</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>468</v>
+        <v>480</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>469</v>
+        <v>481</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>470</v>
+        <v>482</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6841,106 +6935,106 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>471</v>
+        <v>483</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>472</v>
+        <v>484</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>473</v>
+        <v>485</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>474</v>
+        <v>486</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>475</v>
+        <v>487</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>476</v>
+        <v>488</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>477</v>
+        <v>489</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>478</v>
+        <v>490</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>479</v>
+        <v>491</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>480</v>
+        <v>492</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>481</v>
+        <v>493</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>482</v>
+        <v>494</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>483</v>
+        <v>495</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>484</v>
+        <v>496</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>485</v>
+        <v>497</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>486</v>
+        <v>498</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>487</v>
+        <v>499</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>488</v>
+        <v>500</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>489</v>
+        <v>501</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>490</v>
+        <v>502</v>
       </c>
     </row>
   </sheetData>
@@ -6974,822 +7068,822 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>491</v>
+        <v>503</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>430</v>
+        <v>442</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>492</v>
+        <v>504</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>493</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>494</v>
+        <v>505</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>506</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
-        <v>434</v>
+        <v>446</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>435</v>
+        <v>447</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
-        <v>436</v>
+        <v>448</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>437</v>
+        <v>449</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
-        <v>438</v>
+        <v>450</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>495</v>
+        <v>507</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="s">
-        <v>440</v>
+        <v>452</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>496</v>
+        <v>508</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="10" t="s">
-        <v>497</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>498</v>
+        <v>509</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>510</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="s">
-        <v>444</v>
+        <v>456</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>445</v>
+        <v>457</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="10" t="s">
-        <v>446</v>
+        <v>458</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>447</v>
+        <v>459</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="10" t="s">
-        <v>448</v>
+        <v>460</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>499</v>
+        <v>511</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="10" t="s">
-        <v>450</v>
+        <v>462</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>500</v>
+        <v>512</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="10" t="s">
-        <v>501</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>502</v>
+        <v>513</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>514</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="s">
-        <v>454</v>
+        <v>466</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>455</v>
+        <v>467</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="s">
-        <v>456</v>
+        <v>468</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>457</v>
+        <v>469</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="10" t="s">
-        <v>458</v>
+        <v>470</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>503</v>
+        <v>515</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="10" t="s">
-        <v>504</v>
+        <v>516</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>505</v>
+        <v>517</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="10" t="s">
-        <v>506</v>
-      </c>
-      <c r="B23" s="18" t="s">
-        <v>507</v>
+        <v>518</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>519</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="10" t="s">
-        <v>508</v>
+        <v>520</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>509</v>
+        <v>521</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="247.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="10" t="s">
-        <v>510</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>511</v>
+        <v>522</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>523</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="10" t="s">
-        <v>512</v>
+        <v>524</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>513</v>
+        <v>525</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="10" t="s">
-        <v>514</v>
+        <v>526</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>515</v>
+        <v>527</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="10" t="s">
-        <v>516</v>
-      </c>
-      <c r="B29" s="18" t="s">
-        <v>517</v>
+        <v>528</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="10" t="s">
-        <v>518</v>
+        <v>530</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>519</v>
+        <v>531</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="165" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="10" t="s">
-        <v>520</v>
-      </c>
-      <c r="B31" s="13" t="s">
-        <v>521</v>
+        <v>532</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="10" t="s">
-        <v>522</v>
+        <v>534</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>523</v>
+        <v>535</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="10" t="s">
-        <v>524</v>
+        <v>536</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>525</v>
+        <v>537</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="10" t="s">
-        <v>526</v>
-      </c>
-      <c r="B35" s="18" t="s">
-        <v>494</v>
+        <v>538</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>506</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="10" t="s">
-        <v>527</v>
+        <v>539</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>435</v>
+        <v>447</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="10" t="s">
-        <v>528</v>
+        <v>540</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>437</v>
+        <v>449</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="10" t="s">
-        <v>529</v>
+        <v>541</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>530</v>
+        <v>542</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="10" t="s">
-        <v>531</v>
+        <v>543</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>532</v>
+        <v>544</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="10" t="s">
-        <v>533</v>
-      </c>
-      <c r="B41" s="18" t="s">
-        <v>498</v>
+        <v>545</v>
+      </c>
+      <c r="B41" s="19" t="s">
+        <v>510</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="10" t="s">
-        <v>534</v>
+        <v>546</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>445</v>
+        <v>457</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="10" t="s">
-        <v>535</v>
+        <v>547</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>447</v>
+        <v>459</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="10" t="s">
-        <v>536</v>
+        <v>548</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>537</v>
+        <v>549</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="10" t="s">
-        <v>538</v>
+        <v>550</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>539</v>
+        <v>551</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="10" t="s">
-        <v>540</v>
-      </c>
-      <c r="B47" s="18" t="s">
-        <v>502</v>
+        <v>552</v>
+      </c>
+      <c r="B47" s="19" t="s">
+        <v>514</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="10" t="s">
-        <v>541</v>
+        <v>553</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>455</v>
+        <v>467</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="10" t="s">
-        <v>542</v>
+        <v>554</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>457</v>
+        <v>469</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="10" t="s">
-        <v>543</v>
+        <v>555</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>544</v>
+        <v>556</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="10" t="s">
-        <v>545</v>
+        <v>557</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>546</v>
+        <v>558</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="10" t="s">
-        <v>547</v>
-      </c>
-      <c r="B53" s="18" t="s">
-        <v>507</v>
+        <v>559</v>
+      </c>
+      <c r="B53" s="19" t="s">
+        <v>519</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="10" t="s">
-        <v>548</v>
+        <v>560</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>509</v>
+        <v>521</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="247.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="10" t="s">
-        <v>549</v>
-      </c>
-      <c r="B55" s="13" t="s">
-        <v>511</v>
+        <v>561</v>
+      </c>
+      <c r="B55" s="14" t="s">
+        <v>523</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="10" t="s">
-        <v>550</v>
+        <v>562</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>551</v>
+        <v>563</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="10" t="s">
-        <v>552</v>
+        <v>564</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>553</v>
+        <v>565</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="10" t="s">
-        <v>554</v>
-      </c>
-      <c r="B59" s="18" t="s">
-        <v>517</v>
+        <v>566</v>
+      </c>
+      <c r="B59" s="19" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="10" t="s">
-        <v>555</v>
+        <v>567</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>519</v>
+        <v>531</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="165" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="10" t="s">
-        <v>556</v>
-      </c>
-      <c r="B61" s="13" t="s">
-        <v>521</v>
+        <v>568</v>
+      </c>
+      <c r="B61" s="14" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="10" t="s">
-        <v>557</v>
+        <v>569</v>
       </c>
       <c r="B62" s="10" t="s">
-        <v>558</v>
+        <v>570</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="10" t="s">
-        <v>559</v>
+        <v>571</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>560</v>
+        <v>572</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="10" t="s">
-        <v>561</v>
-      </c>
-      <c r="B65" s="18" t="s">
-        <v>494</v>
+        <v>573</v>
+      </c>
+      <c r="B65" s="19" t="s">
+        <v>506</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="10" t="s">
-        <v>562</v>
+        <v>574</v>
       </c>
       <c r="B66" s="10" t="s">
-        <v>435</v>
+        <v>447</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="10" t="s">
-        <v>563</v>
+        <v>575</v>
       </c>
       <c r="B67" s="10" t="s">
-        <v>437</v>
+        <v>449</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="10" t="s">
-        <v>564</v>
+        <v>576</v>
       </c>
       <c r="B68" s="10" t="s">
-        <v>565</v>
+        <v>577</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="10" t="s">
-        <v>566</v>
+        <v>578</v>
       </c>
       <c r="B70" s="10" t="s">
-        <v>567</v>
+        <v>579</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="10" t="s">
-        <v>568</v>
-      </c>
-      <c r="B71" s="18" t="s">
-        <v>569</v>
+        <v>580</v>
+      </c>
+      <c r="B71" s="19" t="s">
+        <v>581</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="10" t="s">
-        <v>570</v>
+        <v>582</v>
       </c>
       <c r="B72" s="10" t="s">
-        <v>445</v>
+        <v>457</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="10" t="s">
-        <v>571</v>
+        <v>583</v>
       </c>
       <c r="B73" s="10" t="s">
-        <v>447</v>
+        <v>459</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="10" t="s">
-        <v>572</v>
+        <v>584</v>
       </c>
       <c r="B74" s="10" t="s">
-        <v>573</v>
+        <v>585</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="10" t="s">
-        <v>574</v>
+        <v>586</v>
       </c>
       <c r="B76" s="10" t="s">
-        <v>575</v>
+        <v>587</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="10" t="s">
-        <v>576</v>
-      </c>
-      <c r="B77" s="18" t="s">
-        <v>577</v>
+        <v>588</v>
+      </c>
+      <c r="B77" s="19" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="10" t="s">
-        <v>578</v>
+        <v>590</v>
       </c>
       <c r="B78" s="10" t="s">
-        <v>455</v>
+        <v>467</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="10" t="s">
-        <v>579</v>
+        <v>591</v>
       </c>
       <c r="B79" s="10" t="s">
-        <v>457</v>
+        <v>469</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="10" t="s">
-        <v>580</v>
+        <v>592</v>
       </c>
       <c r="B80" s="10" t="s">
-        <v>581</v>
+        <v>593</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="10" t="s">
-        <v>582</v>
+        <v>594</v>
       </c>
       <c r="B82" s="10" t="s">
-        <v>583</v>
+        <v>595</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="10" t="s">
-        <v>584</v>
-      </c>
-      <c r="B83" s="18" t="s">
-        <v>585</v>
+        <v>596</v>
+      </c>
+      <c r="B83" s="19" t="s">
+        <v>597</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="10" t="s">
-        <v>586</v>
+        <v>598</v>
       </c>
       <c r="B84" s="10" t="s">
-        <v>509</v>
+        <v>521</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="247.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="10" t="s">
-        <v>587</v>
-      </c>
-      <c r="B85" s="13" t="s">
-        <v>511</v>
+        <v>599</v>
+      </c>
+      <c r="B85" s="14" t="s">
+        <v>523</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="10" t="s">
-        <v>588</v>
+        <v>600</v>
       </c>
       <c r="B86" s="10" t="s">
-        <v>589</v>
+        <v>601</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="10" t="s">
-        <v>590</v>
+        <v>602</v>
       </c>
       <c r="B88" s="10" t="s">
-        <v>591</v>
+        <v>603</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="10" t="s">
-        <v>592</v>
-      </c>
-      <c r="B89" s="18" t="s">
-        <v>593</v>
+        <v>604</v>
+      </c>
+      <c r="B89" s="19" t="s">
+        <v>605</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="10" t="s">
-        <v>594</v>
+        <v>606</v>
       </c>
       <c r="B90" s="10" t="s">
-        <v>519</v>
+        <v>531</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="165" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="10" t="s">
-        <v>595</v>
-      </c>
-      <c r="B91" s="13" t="s">
-        <v>521</v>
+        <v>607</v>
+      </c>
+      <c r="B91" s="14" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="10" t="s">
-        <v>596</v>
+        <v>608</v>
       </c>
       <c r="B92" s="10" t="s">
-        <v>597</v>
+        <v>609</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="10" t="s">
-        <v>598</v>
+        <v>610</v>
       </c>
       <c r="B94" s="10" t="s">
-        <v>599</v>
+        <v>611</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="10" t="s">
-        <v>600</v>
-      </c>
-      <c r="B95" s="18" t="s">
-        <v>569</v>
+        <v>612</v>
+      </c>
+      <c r="B95" s="19" t="s">
+        <v>581</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="10" t="s">
-        <v>601</v>
+        <v>613</v>
       </c>
       <c r="B96" s="10" t="s">
-        <v>435</v>
+        <v>447</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="10" t="s">
-        <v>602</v>
+        <v>614</v>
       </c>
       <c r="B97" s="10" t="s">
-        <v>437</v>
+        <v>449</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="10" t="s">
-        <v>603</v>
+        <v>615</v>
       </c>
       <c r="B98" s="10" t="s">
-        <v>604</v>
+        <v>616</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="10" t="s">
-        <v>605</v>
+        <v>617</v>
       </c>
       <c r="B100" s="10" t="s">
-        <v>606</v>
+        <v>618</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="10" t="s">
-        <v>607</v>
-      </c>
-      <c r="B101" s="18" t="s">
-        <v>608</v>
+        <v>619</v>
+      </c>
+      <c r="B101" s="19" t="s">
+        <v>620</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="10" t="s">
-        <v>609</v>
+        <v>621</v>
       </c>
       <c r="B102" s="10" t="s">
-        <v>445</v>
+        <v>457</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="10" t="s">
-        <v>610</v>
+        <v>622</v>
       </c>
       <c r="B103" s="10" t="s">
-        <v>447</v>
+        <v>459</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="10" t="s">
-        <v>611</v>
+        <v>623</v>
       </c>
       <c r="B104" s="10" t="s">
-        <v>612</v>
+        <v>624</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="10" t="s">
-        <v>613</v>
+        <v>625</v>
       </c>
       <c r="B106" s="10" t="s">
-        <v>614</v>
+        <v>626</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="10" t="s">
-        <v>615</v>
-      </c>
-      <c r="B107" s="18" t="s">
-        <v>616</v>
+        <v>627</v>
+      </c>
+      <c r="B107" s="19" t="s">
+        <v>628</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="10" t="s">
-        <v>617</v>
+        <v>629</v>
       </c>
       <c r="B108" s="10" t="s">
-        <v>455</v>
+        <v>467</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="10" t="s">
-        <v>618</v>
+        <v>630</v>
       </c>
       <c r="B109" s="10" t="s">
-        <v>457</v>
+        <v>469</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="10" t="s">
-        <v>619</v>
+        <v>631</v>
       </c>
       <c r="B110" s="10" t="s">
-        <v>620</v>
+        <v>632</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="10" t="s">
-        <v>621</v>
+        <v>633</v>
       </c>
       <c r="B112" s="10" t="s">
-        <v>622</v>
+        <v>634</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="10" t="s">
-        <v>623</v>
-      </c>
-      <c r="B113" s="18" t="s">
-        <v>507</v>
+        <v>635</v>
+      </c>
+      <c r="B113" s="19" t="s">
+        <v>519</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="10" t="s">
-        <v>624</v>
+        <v>636</v>
       </c>
       <c r="B114" s="10" t="s">
-        <v>509</v>
+        <v>521</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="247.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="10" t="s">
-        <v>625</v>
-      </c>
-      <c r="B115" s="13" t="s">
-        <v>511</v>
+        <v>637</v>
+      </c>
+      <c r="B115" s="14" t="s">
+        <v>523</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="10" t="s">
-        <v>626</v>
+        <v>638</v>
       </c>
       <c r="B116" s="10" t="s">
-        <v>627</v>
+        <v>639</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="10" t="s">
-        <v>628</v>
+        <v>640</v>
       </c>
       <c r="B118" s="10" t="s">
-        <v>629</v>
+        <v>641</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="10" t="s">
-        <v>630</v>
-      </c>
-      <c r="B119" s="18" t="s">
-        <v>517</v>
+        <v>642</v>
+      </c>
+      <c r="B119" s="19" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="10" t="s">
-        <v>631</v>
+        <v>643</v>
       </c>
       <c r="B120" s="10" t="s">
-        <v>519</v>
+        <v>531</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="165" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="10" t="s">
-        <v>632</v>
-      </c>
-      <c r="B121" s="13" t="s">
-        <v>521</v>
+        <v>644</v>
+      </c>
+      <c r="B121" s="14" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="10" t="s">
-        <v>633</v>
+        <v>645</v>
       </c>
       <c r="B122" s="10" t="s">
-        <v>634</v>
+        <v>646</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- About section 1 mobile
</commit_message>
<xml_diff>
--- a/data/text.xlsx
+++ b/data/text.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\ReactJS\_neko_website\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CEDF19E-A23B-46A4-B5D8-839B8962C4B7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C8D03B-B628-4602-96D8-BF089D88CA0E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COMMON" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="779">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="781">
   <si>
     <t>::ID::</t>
   </si>
@@ -3393,6 +3393,135 @@
   </si>
   <si>
     <t>/images/footer/Make_It_Live_Small.png</t>
+  </si>
+  <si>
+    <t>SECTION_1_TEXT_1_SMALL</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">We are
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>&lt;span className='{{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF70AD47"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>custom</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>}}'&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFF26A65"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>the possible match</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;/span&gt;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">for your desire.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>&lt;span className='{{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF70AD47"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>custom</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>}}'&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFF26A65"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Don't you realise it?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>&lt;/span</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -5257,7 +5386,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
@@ -7111,10 +7240,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7143,169 +7272,177 @@
         <v>485</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="2"/>
+    <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>779</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>780</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>486</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>488</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B6" s="10" t="s">
         <v>489</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>490</v>
-      </c>
-      <c r="B6" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>492</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>493</v>
+        <v>490</v>
+      </c>
+      <c r="B7" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>492</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>494</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B9" s="10" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="10"/>
-    </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B10" s="10"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>496</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>498</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B12" s="10" t="s">
         <v>499</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>500</v>
-      </c>
-      <c r="B12" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>501</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>362</v>
+        <v>500</v>
+      </c>
+      <c r="B13" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>501</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>502</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B15" s="10" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>366</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B16" s="10" t="s">
         <v>504</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>374</v>
-      </c>
-      <c r="B17" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>374</v>
+      </c>
+      <c r="B18" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>384</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>394</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B20" s="10" t="s">
         <v>507</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>508</v>
-      </c>
-      <c r="B21" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="B22" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B23" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B24" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B25" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>516</v>
+      </c>
+      <c r="B26" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>518</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>519</v>
       </c>
     </row>

</xml_diff>

<commit_message>
* about contact mobile
</commit_message>
<xml_diff>
--- a/data/text.xlsx
+++ b/data/text.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\ReactJS\_neko_website\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C8D03B-B628-4602-96D8-BF089D88CA0E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E53E82F5-800C-4CD4-BAE1-96ACB38BE9F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7242,7 +7242,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
* Capabilities mobile section 1
</commit_message>
<xml_diff>
--- a/data/text.xlsx
+++ b/data/text.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\ReactJS\_neko_website\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E53E82F5-800C-4CD4-BAE1-96ACB38BE9F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0EADF85-3418-49B1-AA72-F2D24290EEB4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COMMON" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="781">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="782">
   <si>
     <t>::ID::</t>
   </si>
@@ -3521,6 +3521,62 @@
         <charset val="1"/>
       </rPr>
       <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;span className='{{</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF70AD47"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>custom</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>}}'&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFED7D31"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Good design</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;/span&gt;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>make perfect sense
+to your goal.</t>
     </r>
   </si>
 </sst>
@@ -4165,9 +4221,11 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4195,219 +4253,227 @@
         <v>664</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>779</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
         <v>455</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B5" s="15" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
         <v>459</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B6" s="10" t="s">
         <v>666</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
         <v>667</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B7" s="10" t="s">
         <v>668</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>669</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>670</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
+        <v>669</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
         <v>463</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B9" s="10" t="s">
         <v>671</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
         <v>465</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B11" s="15" t="s">
         <v>672</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
         <v>469</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B12" s="10" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
         <v>673</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B13" s="10" t="s">
         <v>674</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
-        <v>675</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>676</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
+        <v>675</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
         <v>473</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B15" s="10" t="s">
         <v>677</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="19" t="s">
         <v>475</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B17" s="15" t="s">
         <v>678</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
         <v>479</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B18" s="10" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
+    <row r="19" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
         <v>679</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B19" s="10" t="s">
         <v>680</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
-        <v>681</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>682</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
+        <v>681</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
         <v>483</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B21" s="10" t="s">
         <v>683</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="19" t="s">
         <v>533</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B23" s="15" t="s">
         <v>684</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="15" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
         <v>537</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B24" s="10" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
+    <row r="25" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
         <v>685</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B25" s="10" t="s">
         <v>686</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="15" t="s">
-        <v>687</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>688</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
+        <v>687</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
         <v>541</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B27" s="10" t="s">
         <v>689</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="19" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="19" t="s">
         <v>543</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B29" s="15" t="s">
         <v>690</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="15" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
         <v>547</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B30" s="10" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="15" t="s">
+    <row r="31" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="15" t="s">
         <v>691</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B31" s="10" t="s">
         <v>692</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="15" t="s">
-        <v>693</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>694</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
+        <v>693</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="15" t="s">
         <v>551</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="B33" s="10" t="s">
         <v>695</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>696</v>
-      </c>
-      <c r="B34" t="s">
-        <v>697</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>696</v>
+      </c>
+      <c r="B35" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>698</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>362</v>
       </c>
     </row>
@@ -7242,7 +7308,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>